<commit_message>
Add bypass capacitors for 3V3
</commit_message>
<xml_diff>
--- a/BOM/XUF208_Breakout_BOM.xlsx
+++ b/BOM/XUF208_Breakout_BOM.xlsx
@@ -3,12 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="XUF208_Breakout_BOM" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="XUF208_Breakout" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName localSheetId="0" name="Print_Titles">XUF208_Breakout_BOM!$1:$1</definedName>
+    <definedName localSheetId="0" name="Print_Titles">XUF208_Breakout!$1:$1</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -41,7 +39,7 @@
     <t>Manufacturer Part Number</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C17</t>
+    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C19</t>
   </si>
   <si>
     <t>100nF</t>
@@ -59,7 +57,7 @@
     <t>CL10B104KB8NNNC</t>
   </si>
   <si>
-    <t>C10</t>
+    <t>C12</t>
   </si>
   <si>
     <t>1uF</t>
@@ -68,7 +66,7 @@
     <t>CL10A105KB8NNNC</t>
   </si>
   <si>
-    <t>C11, C12, C14, C15</t>
+    <t>C13, C14, C16, C17</t>
   </si>
   <si>
     <t>10uF</t>
@@ -77,7 +75,7 @@
     <t>CL10A106MQ8NNNC</t>
   </si>
   <si>
-    <t>C13, C16</t>
+    <t>C15, C18</t>
   </si>
   <si>
     <t>10nF</t>
@@ -329,7 +327,7 @@
     <t>RC0603FR-075K1L</t>
   </si>
   <si>
-    <t>RESET</t>
+    <t>RESET1</t>
   </si>
   <si>
     <t>Switch</t>
@@ -356,7 +354,7 @@
     <t>TQ64</t>
   </si>
   <si>
-    <t>U2(optional)</t>
+    <t>U2</t>
   </si>
   <si>
     <t>3V 16M-BIT SERIAL FLASH MEMORY WITH DUAL/QUAD SPI</t>
@@ -432,10 +430,10 @@
     </font>
     <font/>
     <font>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
     </font>
   </fonts>
@@ -453,7 +451,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border/>
     <border>
       <left style="thin">
@@ -500,11 +498,16 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -523,23 +526,26 @@
     <xf quotePrefix="1" borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf quotePrefix="1" borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf quotePrefix="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,14 +556,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -766,9 +764,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="8.14"/>
-    <col customWidth="1" min="2" max="2" width="33.71"/>
+    <col customWidth="1" min="2" max="2" width="42.29"/>
     <col customWidth="1" min="3" max="3" width="18.29"/>
-    <col customWidth="1" min="4" max="4" width="31.14"/>
+    <col customWidth="1" min="4" max="4" width="33.71"/>
     <col customWidth="1" min="5" max="6" width="19.86"/>
     <col customWidth="1" min="7" max="7" width="21.43"/>
     <col customWidth="1" min="8" max="8" width="26.86"/>
@@ -821,7 +819,7 @@
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="4">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
@@ -885,7 +883,7 @@
       <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="3"/>
@@ -929,7 +927,7 @@
       <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="3"/>
@@ -973,7 +971,7 @@
       <c r="G5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
@@ -1002,7 +1000,7 @@
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="5" t="s">
         <v>24</v>
       </c>
@@ -1015,7 +1013,7 @@
       <c r="G6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="3"/>
@@ -1044,7 +1042,7 @@
       <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1057,7 +1055,7 @@
       <c r="G7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>32</v>
       </c>
       <c r="I7" s="3"/>
@@ -1086,7 +1084,7 @@
       <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="5" t="s">
         <v>34</v>
       </c>
@@ -1099,7 +1097,7 @@
       <c r="G8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I8" s="3"/>
@@ -1122,13 +1120,13 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="4">
-        <v>2.0</v>
+      <c r="A9" s="9">
+        <v>1.0</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1143,7 +1141,7 @@
       <c r="G9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="7" t="s">
         <v>43</v>
       </c>
       <c r="I9" s="3"/>
@@ -1166,13 +1164,13 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="4">
-        <v>2.0</v>
+      <c r="A10" s="9">
+        <v>1.0</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1187,7 +1185,7 @@
       <c r="G10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I10" s="3"/>
@@ -1216,7 +1214,7 @@
       <c r="B11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="5" t="s">
         <v>48</v>
       </c>
@@ -1229,7 +1227,7 @@
       <c r="G11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="7" t="s">
         <v>51</v>
       </c>
       <c r="I11" s="3"/>
@@ -1258,7 +1256,7 @@
       <c r="B12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="5" t="s">
         <v>53</v>
       </c>
@@ -1271,7 +1269,7 @@
       <c r="G12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="7" t="s">
         <v>56</v>
       </c>
       <c r="I12" s="3"/>
@@ -1300,7 +1298,7 @@
       <c r="B13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="5" t="s">
         <v>58</v>
       </c>
@@ -1313,7 +1311,7 @@
       <c r="G13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1340,7 +1338,7 @@
       <c r="B14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
@@ -1353,7 +1351,7 @@
       <c r="G14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1395,7 +1393,7 @@
       <c r="G15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="11" t="s">
         <v>70</v>
       </c>
       <c r="I15" s="3"/>
@@ -1439,7 +1437,7 @@
       <c r="G16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="7" t="s">
         <v>73</v>
       </c>
       <c r="I16" s="3"/>
@@ -1483,7 +1481,7 @@
       <c r="G17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="7" t="s">
         <v>76</v>
       </c>
       <c r="I17" s="3"/>
@@ -1527,7 +1525,7 @@
       <c r="G18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="7" t="s">
         <v>79</v>
       </c>
       <c r="I18" s="3"/>
@@ -1571,7 +1569,7 @@
       <c r="G19" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="7" t="s">
         <v>82</v>
       </c>
       <c r="I19" s="3"/>
@@ -1615,7 +1613,7 @@
       <c r="G20" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="7" t="s">
         <v>85</v>
       </c>
       <c r="I20" s="3"/>
@@ -1659,7 +1657,7 @@
       <c r="G21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="7" t="s">
         <v>88</v>
       </c>
       <c r="I21" s="3"/>
@@ -1703,7 +1701,7 @@
       <c r="G22" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="7" t="s">
         <v>91</v>
       </c>
       <c r="I22" s="3"/>
@@ -1747,7 +1745,7 @@
       <c r="G23" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="7" t="s">
         <v>94</v>
       </c>
       <c r="I23" s="3"/>
@@ -1791,7 +1789,7 @@
       <c r="G24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="7" t="s">
         <v>97</v>
       </c>
       <c r="I24" s="3"/>
@@ -1835,7 +1833,7 @@
       <c r="G25" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="7" t="s">
         <v>100</v>
       </c>
       <c r="I25" s="3"/>
@@ -1879,7 +1877,7 @@
       <c r="G26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="7" t="s">
         <v>103</v>
       </c>
       <c r="I26" s="3"/>
@@ -1908,7 +1906,7 @@
       <c r="B27" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="7"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="5" t="s">
         <v>105</v>
       </c>
@@ -1921,7 +1919,7 @@
       <c r="G27" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I27" s="3"/>
@@ -1950,7 +1948,7 @@
       <c r="B28" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="7"/>
+      <c r="C28" s="8"/>
       <c r="D28" s="5" t="s">
         <v>110</v>
       </c>
@@ -1963,7 +1961,7 @@
       <c r="G28" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="12" t="s">
         <v>111</v>
       </c>
       <c r="I28" s="3"/>
@@ -1989,10 +1987,10 @@
       <c r="A29" s="4">
         <v>1.0</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="7"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="5" t="s">
         <v>114</v>
       </c>
@@ -2005,7 +2003,7 @@
       <c r="G29" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="7" t="s">
         <v>117</v>
       </c>
       <c r="I29" s="3"/>
@@ -2034,7 +2032,7 @@
       <c r="B30" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="7"/>
+      <c r="C30" s="8"/>
       <c r="D30" s="5" t="s">
         <v>119</v>
       </c>
@@ -2047,7 +2045,7 @@
       <c r="G30" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="7" t="s">
         <v>122</v>
       </c>
       <c r="I30" s="3"/>
@@ -2076,7 +2074,7 @@
       <c r="B31" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C31" s="7"/>
+      <c r="C31" s="8"/>
       <c r="D31" s="5" t="s">
         <v>124</v>
       </c>
@@ -2089,7 +2087,7 @@
       <c r="G31" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="7" t="s">
         <v>127</v>
       </c>
       <c r="I31" s="3"/>
@@ -2118,7 +2116,7 @@
       <c r="B32" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C32" s="7"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="5" t="s">
         <v>129</v>
       </c>
@@ -2131,7 +2129,7 @@
       <c r="G32" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="7" t="s">
         <v>132</v>
       </c>
       <c r="I32" s="3"/>
@@ -29235,2046 +29233,4 @@
   <pageSetup paperSize="9" orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="26" width="0.71"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="12.75" customHeight="1"/>
-    <row r="2" ht="12.75" customHeight="1"/>
-    <row r="3" ht="12.75" customHeight="1"/>
-    <row r="4" ht="12.75" customHeight="1"/>
-    <row r="5" ht="12.75" customHeight="1"/>
-    <row r="6" ht="12.75" customHeight="1"/>
-    <row r="7" ht="12.75" customHeight="1"/>
-    <row r="8" ht="12.75" customHeight="1"/>
-    <row r="9" ht="12.75" customHeight="1"/>
-    <row r="10" ht="12.75" customHeight="1"/>
-    <row r="11" ht="12.75" customHeight="1"/>
-    <row r="12" ht="12.75" customHeight="1"/>
-    <row r="13" ht="12.75" customHeight="1"/>
-    <row r="14" ht="12.75" customHeight="1"/>
-    <row r="15" ht="12.75" customHeight="1"/>
-    <row r="16" ht="12.75" customHeight="1"/>
-    <row r="17" ht="12.75" customHeight="1"/>
-    <row r="18" ht="12.75" customHeight="1"/>
-    <row r="19" ht="12.75" customHeight="1"/>
-    <row r="20" ht="12.75" customHeight="1"/>
-    <row r="21" ht="12.75" customHeight="1"/>
-    <row r="22" ht="12.75" customHeight="1"/>
-    <row r="23" ht="12.75" customHeight="1"/>
-    <row r="24" ht="12.75" customHeight="1"/>
-    <row r="25" ht="12.75" customHeight="1"/>
-    <row r="26" ht="12.75" customHeight="1"/>
-    <row r="27" ht="12.75" customHeight="1"/>
-    <row r="28" ht="12.75" customHeight="1"/>
-    <row r="29" ht="12.75" customHeight="1"/>
-    <row r="30" ht="12.75" customHeight="1"/>
-    <row r="31" ht="12.75" customHeight="1"/>
-    <row r="32" ht="12.75" customHeight="1"/>
-    <row r="33" ht="12.75" customHeight="1"/>
-    <row r="34" ht="12.75" customHeight="1"/>
-    <row r="35" ht="12.75" customHeight="1"/>
-    <row r="36" ht="12.75" customHeight="1"/>
-    <row r="37" ht="12.75" customHeight="1"/>
-    <row r="38" ht="12.75" customHeight="1"/>
-    <row r="39" ht="12.75" customHeight="1"/>
-    <row r="40" ht="12.75" customHeight="1"/>
-    <row r="41" ht="12.75" customHeight="1"/>
-    <row r="42" ht="12.75" customHeight="1"/>
-    <row r="43" ht="12.75" customHeight="1"/>
-    <row r="44" ht="12.75" customHeight="1"/>
-    <row r="45" ht="12.75" customHeight="1"/>
-    <row r="46" ht="12.75" customHeight="1"/>
-    <row r="47" ht="12.75" customHeight="1"/>
-    <row r="48" ht="12.75" customHeight="1"/>
-    <row r="49" ht="12.75" customHeight="1"/>
-    <row r="50" ht="12.75" customHeight="1"/>
-    <row r="51" ht="12.75" customHeight="1"/>
-    <row r="52" ht="12.75" customHeight="1"/>
-    <row r="53" ht="12.75" customHeight="1"/>
-    <row r="54" ht="12.75" customHeight="1"/>
-    <row r="55" ht="12.75" customHeight="1"/>
-    <row r="56" ht="12.75" customHeight="1"/>
-    <row r="57" ht="12.75" customHeight="1"/>
-    <row r="58" ht="12.75" customHeight="1"/>
-    <row r="59" ht="12.75" customHeight="1"/>
-    <row r="60" ht="12.75" customHeight="1"/>
-    <row r="61" ht="12.75" customHeight="1"/>
-    <row r="62" ht="12.75" customHeight="1"/>
-    <row r="63" ht="12.75" customHeight="1"/>
-    <row r="64" ht="12.75" customHeight="1"/>
-    <row r="65" ht="12.75" customHeight="1"/>
-    <row r="66" ht="12.75" customHeight="1"/>
-    <row r="67" ht="12.75" customHeight="1"/>
-    <row r="68" ht="12.75" customHeight="1"/>
-    <row r="69" ht="12.75" customHeight="1"/>
-    <row r="70" ht="12.75" customHeight="1"/>
-    <row r="71" ht="12.75" customHeight="1"/>
-    <row r="72" ht="12.75" customHeight="1"/>
-    <row r="73" ht="12.75" customHeight="1"/>
-    <row r="74" ht="12.75" customHeight="1"/>
-    <row r="75" ht="12.75" customHeight="1"/>
-    <row r="76" ht="12.75" customHeight="1"/>
-    <row r="77" ht="12.75" customHeight="1"/>
-    <row r="78" ht="12.75" customHeight="1"/>
-    <row r="79" ht="12.75" customHeight="1"/>
-    <row r="80" ht="12.75" customHeight="1"/>
-    <row r="81" ht="12.75" customHeight="1"/>
-    <row r="82" ht="12.75" customHeight="1"/>
-    <row r="83" ht="12.75" customHeight="1"/>
-    <row r="84" ht="12.75" customHeight="1"/>
-    <row r="85" ht="12.75" customHeight="1"/>
-    <row r="86" ht="12.75" customHeight="1"/>
-    <row r="87" ht="12.75" customHeight="1"/>
-    <row r="88" ht="12.75" customHeight="1"/>
-    <row r="89" ht="12.75" customHeight="1"/>
-    <row r="90" ht="12.75" customHeight="1"/>
-    <row r="91" ht="12.75" customHeight="1"/>
-    <row r="92" ht="12.75" customHeight="1"/>
-    <row r="93" ht="12.75" customHeight="1"/>
-    <row r="94" ht="12.75" customHeight="1"/>
-    <row r="95" ht="12.75" customHeight="1"/>
-    <row r="96" ht="12.75" customHeight="1"/>
-    <row r="97" ht="12.75" customHeight="1"/>
-    <row r="98" ht="12.75" customHeight="1"/>
-    <row r="99" ht="12.75" customHeight="1"/>
-    <row r="100" ht="12.75" customHeight="1"/>
-    <row r="101" ht="12.75" customHeight="1"/>
-    <row r="102" ht="12.75" customHeight="1"/>
-    <row r="103" ht="12.75" customHeight="1"/>
-    <row r="104" ht="12.75" customHeight="1"/>
-    <row r="105" ht="12.75" customHeight="1"/>
-    <row r="106" ht="12.75" customHeight="1"/>
-    <row r="107" ht="12.75" customHeight="1"/>
-    <row r="108" ht="12.75" customHeight="1"/>
-    <row r="109" ht="12.75" customHeight="1"/>
-    <row r="110" ht="12.75" customHeight="1"/>
-    <row r="111" ht="12.75" customHeight="1"/>
-    <row r="112" ht="12.75" customHeight="1"/>
-    <row r="113" ht="12.75" customHeight="1"/>
-    <row r="114" ht="12.75" customHeight="1"/>
-    <row r="115" ht="12.75" customHeight="1"/>
-    <row r="116" ht="12.75" customHeight="1"/>
-    <row r="117" ht="12.75" customHeight="1"/>
-    <row r="118" ht="12.75" customHeight="1"/>
-    <row r="119" ht="12.75" customHeight="1"/>
-    <row r="120" ht="12.75" customHeight="1"/>
-    <row r="121" ht="12.75" customHeight="1"/>
-    <row r="122" ht="12.75" customHeight="1"/>
-    <row r="123" ht="12.75" customHeight="1"/>
-    <row r="124" ht="12.75" customHeight="1"/>
-    <row r="125" ht="12.75" customHeight="1"/>
-    <row r="126" ht="12.75" customHeight="1"/>
-    <row r="127" ht="12.75" customHeight="1"/>
-    <row r="128" ht="12.75" customHeight="1"/>
-    <row r="129" ht="12.75" customHeight="1"/>
-    <row r="130" ht="12.75" customHeight="1"/>
-    <row r="131" ht="12.75" customHeight="1"/>
-    <row r="132" ht="12.75" customHeight="1"/>
-    <row r="133" ht="12.75" customHeight="1"/>
-    <row r="134" ht="12.75" customHeight="1"/>
-    <row r="135" ht="12.75" customHeight="1"/>
-    <row r="136" ht="12.75" customHeight="1"/>
-    <row r="137" ht="12.75" customHeight="1"/>
-    <row r="138" ht="12.75" customHeight="1"/>
-    <row r="139" ht="12.75" customHeight="1"/>
-    <row r="140" ht="12.75" customHeight="1"/>
-    <row r="141" ht="12.75" customHeight="1"/>
-    <row r="142" ht="12.75" customHeight="1"/>
-    <row r="143" ht="12.75" customHeight="1"/>
-    <row r="144" ht="12.75" customHeight="1"/>
-    <row r="145" ht="12.75" customHeight="1"/>
-    <row r="146" ht="12.75" customHeight="1"/>
-    <row r="147" ht="12.75" customHeight="1"/>
-    <row r="148" ht="12.75" customHeight="1"/>
-    <row r="149" ht="12.75" customHeight="1"/>
-    <row r="150" ht="12.75" customHeight="1"/>
-    <row r="151" ht="12.75" customHeight="1"/>
-    <row r="152" ht="12.75" customHeight="1"/>
-    <row r="153" ht="12.75" customHeight="1"/>
-    <row r="154" ht="12.75" customHeight="1"/>
-    <row r="155" ht="12.75" customHeight="1"/>
-    <row r="156" ht="12.75" customHeight="1"/>
-    <row r="157" ht="12.75" customHeight="1"/>
-    <row r="158" ht="12.75" customHeight="1"/>
-    <row r="159" ht="12.75" customHeight="1"/>
-    <row r="160" ht="12.75" customHeight="1"/>
-    <row r="161" ht="12.75" customHeight="1"/>
-    <row r="162" ht="12.75" customHeight="1"/>
-    <row r="163" ht="12.75" customHeight="1"/>
-    <row r="164" ht="12.75" customHeight="1"/>
-    <row r="165" ht="12.75" customHeight="1"/>
-    <row r="166" ht="12.75" customHeight="1"/>
-    <row r="167" ht="12.75" customHeight="1"/>
-    <row r="168" ht="12.75" customHeight="1"/>
-    <row r="169" ht="12.75" customHeight="1"/>
-    <row r="170" ht="12.75" customHeight="1"/>
-    <row r="171" ht="12.75" customHeight="1"/>
-    <row r="172" ht="12.75" customHeight="1"/>
-    <row r="173" ht="12.75" customHeight="1"/>
-    <row r="174" ht="12.75" customHeight="1"/>
-    <row r="175" ht="12.75" customHeight="1"/>
-    <row r="176" ht="12.75" customHeight="1"/>
-    <row r="177" ht="12.75" customHeight="1"/>
-    <row r="178" ht="12.75" customHeight="1"/>
-    <row r="179" ht="12.75" customHeight="1"/>
-    <row r="180" ht="12.75" customHeight="1"/>
-    <row r="181" ht="12.75" customHeight="1"/>
-    <row r="182" ht="12.75" customHeight="1"/>
-    <row r="183" ht="12.75" customHeight="1"/>
-    <row r="184" ht="12.75" customHeight="1"/>
-    <row r="185" ht="12.75" customHeight="1"/>
-    <row r="186" ht="12.75" customHeight="1"/>
-    <row r="187" ht="12.75" customHeight="1"/>
-    <row r="188" ht="12.75" customHeight="1"/>
-    <row r="189" ht="12.75" customHeight="1"/>
-    <row r="190" ht="12.75" customHeight="1"/>
-    <row r="191" ht="12.75" customHeight="1"/>
-    <row r="192" ht="12.75" customHeight="1"/>
-    <row r="193" ht="12.75" customHeight="1"/>
-    <row r="194" ht="12.75" customHeight="1"/>
-    <row r="195" ht="12.75" customHeight="1"/>
-    <row r="196" ht="12.75" customHeight="1"/>
-    <row r="197" ht="12.75" customHeight="1"/>
-    <row r="198" ht="12.75" customHeight="1"/>
-    <row r="199" ht="12.75" customHeight="1"/>
-    <row r="200" ht="12.75" customHeight="1"/>
-    <row r="201" ht="12.75" customHeight="1"/>
-    <row r="202" ht="12.75" customHeight="1"/>
-    <row r="203" ht="12.75" customHeight="1"/>
-    <row r="204" ht="12.75" customHeight="1"/>
-    <row r="205" ht="12.75" customHeight="1"/>
-    <row r="206" ht="12.75" customHeight="1"/>
-    <row r="207" ht="12.75" customHeight="1"/>
-    <row r="208" ht="12.75" customHeight="1"/>
-    <row r="209" ht="12.75" customHeight="1"/>
-    <row r="210" ht="12.75" customHeight="1"/>
-    <row r="211" ht="12.75" customHeight="1"/>
-    <row r="212" ht="12.75" customHeight="1"/>
-    <row r="213" ht="12.75" customHeight="1"/>
-    <row r="214" ht="12.75" customHeight="1"/>
-    <row r="215" ht="12.75" customHeight="1"/>
-    <row r="216" ht="12.75" customHeight="1"/>
-    <row r="217" ht="12.75" customHeight="1"/>
-    <row r="218" ht="12.75" customHeight="1"/>
-    <row r="219" ht="12.75" customHeight="1"/>
-    <row r="220" ht="12.75" customHeight="1"/>
-    <row r="221" ht="12.75" customHeight="1"/>
-    <row r="222" ht="12.75" customHeight="1"/>
-    <row r="223" ht="12.75" customHeight="1"/>
-    <row r="224" ht="12.75" customHeight="1"/>
-    <row r="225" ht="12.75" customHeight="1"/>
-    <row r="226" ht="12.75" customHeight="1"/>
-    <row r="227" ht="12.75" customHeight="1"/>
-    <row r="228" ht="12.75" customHeight="1"/>
-    <row r="229" ht="12.75" customHeight="1"/>
-    <row r="230" ht="12.75" customHeight="1"/>
-    <row r="231" ht="12.75" customHeight="1"/>
-    <row r="232" ht="12.75" customHeight="1"/>
-    <row r="233" ht="12.75" customHeight="1"/>
-    <row r="234" ht="12.75" customHeight="1"/>
-    <row r="235" ht="12.75" customHeight="1"/>
-    <row r="236" ht="12.75" customHeight="1"/>
-    <row r="237" ht="12.75" customHeight="1"/>
-    <row r="238" ht="12.75" customHeight="1"/>
-    <row r="239" ht="12.75" customHeight="1"/>
-    <row r="240" ht="12.75" customHeight="1"/>
-    <row r="241" ht="12.75" customHeight="1"/>
-    <row r="242" ht="12.75" customHeight="1"/>
-    <row r="243" ht="12.75" customHeight="1"/>
-    <row r="244" ht="12.75" customHeight="1"/>
-    <row r="245" ht="12.75" customHeight="1"/>
-    <row r="246" ht="12.75" customHeight="1"/>
-    <row r="247" ht="12.75" customHeight="1"/>
-    <row r="248" ht="12.75" customHeight="1"/>
-    <row r="249" ht="12.75" customHeight="1"/>
-    <row r="250" ht="12.75" customHeight="1"/>
-    <row r="251" ht="12.75" customHeight="1"/>
-    <row r="252" ht="12.75" customHeight="1"/>
-    <row r="253" ht="12.75" customHeight="1"/>
-    <row r="254" ht="12.75" customHeight="1"/>
-    <row r="255" ht="12.75" customHeight="1"/>
-    <row r="256" ht="12.75" customHeight="1"/>
-    <row r="257" ht="12.75" customHeight="1"/>
-    <row r="258" ht="12.75" customHeight="1"/>
-    <row r="259" ht="12.75" customHeight="1"/>
-    <row r="260" ht="12.75" customHeight="1"/>
-    <row r="261" ht="12.75" customHeight="1"/>
-    <row r="262" ht="12.75" customHeight="1"/>
-    <row r="263" ht="12.75" customHeight="1"/>
-    <row r="264" ht="12.75" customHeight="1"/>
-    <row r="265" ht="12.75" customHeight="1"/>
-    <row r="266" ht="12.75" customHeight="1"/>
-    <row r="267" ht="12.75" customHeight="1"/>
-    <row r="268" ht="12.75" customHeight="1"/>
-    <row r="269" ht="12.75" customHeight="1"/>
-    <row r="270" ht="12.75" customHeight="1"/>
-    <row r="271" ht="12.75" customHeight="1"/>
-    <row r="272" ht="12.75" customHeight="1"/>
-    <row r="273" ht="12.75" customHeight="1"/>
-    <row r="274" ht="12.75" customHeight="1"/>
-    <row r="275" ht="12.75" customHeight="1"/>
-    <row r="276" ht="12.75" customHeight="1"/>
-    <row r="277" ht="12.75" customHeight="1"/>
-    <row r="278" ht="12.75" customHeight="1"/>
-    <row r="279" ht="12.75" customHeight="1"/>
-    <row r="280" ht="12.75" customHeight="1"/>
-    <row r="281" ht="12.75" customHeight="1"/>
-    <row r="282" ht="12.75" customHeight="1"/>
-    <row r="283" ht="12.75" customHeight="1"/>
-    <row r="284" ht="12.75" customHeight="1"/>
-    <row r="285" ht="12.75" customHeight="1"/>
-    <row r="286" ht="12.75" customHeight="1"/>
-    <row r="287" ht="12.75" customHeight="1"/>
-    <row r="288" ht="12.75" customHeight="1"/>
-    <row r="289" ht="12.75" customHeight="1"/>
-    <row r="290" ht="12.75" customHeight="1"/>
-    <row r="291" ht="12.75" customHeight="1"/>
-    <row r="292" ht="12.75" customHeight="1"/>
-    <row r="293" ht="12.75" customHeight="1"/>
-    <row r="294" ht="12.75" customHeight="1"/>
-    <row r="295" ht="12.75" customHeight="1"/>
-    <row r="296" ht="12.75" customHeight="1"/>
-    <row r="297" ht="12.75" customHeight="1"/>
-    <row r="298" ht="12.75" customHeight="1"/>
-    <row r="299" ht="12.75" customHeight="1"/>
-    <row r="300" ht="12.75" customHeight="1"/>
-    <row r="301" ht="12.75" customHeight="1"/>
-    <row r="302" ht="12.75" customHeight="1"/>
-    <row r="303" ht="12.75" customHeight="1"/>
-    <row r="304" ht="12.75" customHeight="1"/>
-    <row r="305" ht="12.75" customHeight="1"/>
-    <row r="306" ht="12.75" customHeight="1"/>
-    <row r="307" ht="12.75" customHeight="1"/>
-    <row r="308" ht="12.75" customHeight="1"/>
-    <row r="309" ht="12.75" customHeight="1"/>
-    <row r="310" ht="12.75" customHeight="1"/>
-    <row r="311" ht="12.75" customHeight="1"/>
-    <row r="312" ht="12.75" customHeight="1"/>
-    <row r="313" ht="12.75" customHeight="1"/>
-    <row r="314" ht="12.75" customHeight="1"/>
-    <row r="315" ht="12.75" customHeight="1"/>
-    <row r="316" ht="12.75" customHeight="1"/>
-    <row r="317" ht="12.75" customHeight="1"/>
-    <row r="318" ht="12.75" customHeight="1"/>
-    <row r="319" ht="12.75" customHeight="1"/>
-    <row r="320" ht="12.75" customHeight="1"/>
-    <row r="321" ht="12.75" customHeight="1"/>
-    <row r="322" ht="12.75" customHeight="1"/>
-    <row r="323" ht="12.75" customHeight="1"/>
-    <row r="324" ht="12.75" customHeight="1"/>
-    <row r="325" ht="12.75" customHeight="1"/>
-    <row r="326" ht="12.75" customHeight="1"/>
-    <row r="327" ht="12.75" customHeight="1"/>
-    <row r="328" ht="12.75" customHeight="1"/>
-    <row r="329" ht="12.75" customHeight="1"/>
-    <row r="330" ht="12.75" customHeight="1"/>
-    <row r="331" ht="12.75" customHeight="1"/>
-    <row r="332" ht="12.75" customHeight="1"/>
-    <row r="333" ht="12.75" customHeight="1"/>
-    <row r="334" ht="12.75" customHeight="1"/>
-    <row r="335" ht="12.75" customHeight="1"/>
-    <row r="336" ht="12.75" customHeight="1"/>
-    <row r="337" ht="12.75" customHeight="1"/>
-    <row r="338" ht="12.75" customHeight="1"/>
-    <row r="339" ht="12.75" customHeight="1"/>
-    <row r="340" ht="12.75" customHeight="1"/>
-    <row r="341" ht="12.75" customHeight="1"/>
-    <row r="342" ht="12.75" customHeight="1"/>
-    <row r="343" ht="12.75" customHeight="1"/>
-    <row r="344" ht="12.75" customHeight="1"/>
-    <row r="345" ht="12.75" customHeight="1"/>
-    <row r="346" ht="12.75" customHeight="1"/>
-    <row r="347" ht="12.75" customHeight="1"/>
-    <row r="348" ht="12.75" customHeight="1"/>
-    <row r="349" ht="12.75" customHeight="1"/>
-    <row r="350" ht="12.75" customHeight="1"/>
-    <row r="351" ht="12.75" customHeight="1"/>
-    <row r="352" ht="12.75" customHeight="1"/>
-    <row r="353" ht="12.75" customHeight="1"/>
-    <row r="354" ht="12.75" customHeight="1"/>
-    <row r="355" ht="12.75" customHeight="1"/>
-    <row r="356" ht="12.75" customHeight="1"/>
-    <row r="357" ht="12.75" customHeight="1"/>
-    <row r="358" ht="12.75" customHeight="1"/>
-    <row r="359" ht="12.75" customHeight="1"/>
-    <row r="360" ht="12.75" customHeight="1"/>
-    <row r="361" ht="12.75" customHeight="1"/>
-    <row r="362" ht="12.75" customHeight="1"/>
-    <row r="363" ht="12.75" customHeight="1"/>
-    <row r="364" ht="12.75" customHeight="1"/>
-    <row r="365" ht="12.75" customHeight="1"/>
-    <row r="366" ht="12.75" customHeight="1"/>
-    <row r="367" ht="12.75" customHeight="1"/>
-    <row r="368" ht="12.75" customHeight="1"/>
-    <row r="369" ht="12.75" customHeight="1"/>
-    <row r="370" ht="12.75" customHeight="1"/>
-    <row r="371" ht="12.75" customHeight="1"/>
-    <row r="372" ht="12.75" customHeight="1"/>
-    <row r="373" ht="12.75" customHeight="1"/>
-    <row r="374" ht="12.75" customHeight="1"/>
-    <row r="375" ht="12.75" customHeight="1"/>
-    <row r="376" ht="12.75" customHeight="1"/>
-    <row r="377" ht="12.75" customHeight="1"/>
-    <row r="378" ht="12.75" customHeight="1"/>
-    <row r="379" ht="12.75" customHeight="1"/>
-    <row r="380" ht="12.75" customHeight="1"/>
-    <row r="381" ht="12.75" customHeight="1"/>
-    <row r="382" ht="12.75" customHeight="1"/>
-    <row r="383" ht="12.75" customHeight="1"/>
-    <row r="384" ht="12.75" customHeight="1"/>
-    <row r="385" ht="12.75" customHeight="1"/>
-    <row r="386" ht="12.75" customHeight="1"/>
-    <row r="387" ht="12.75" customHeight="1"/>
-    <row r="388" ht="12.75" customHeight="1"/>
-    <row r="389" ht="12.75" customHeight="1"/>
-    <row r="390" ht="12.75" customHeight="1"/>
-    <row r="391" ht="12.75" customHeight="1"/>
-    <row r="392" ht="12.75" customHeight="1"/>
-    <row r="393" ht="12.75" customHeight="1"/>
-    <row r="394" ht="12.75" customHeight="1"/>
-    <row r="395" ht="12.75" customHeight="1"/>
-    <row r="396" ht="12.75" customHeight="1"/>
-    <row r="397" ht="12.75" customHeight="1"/>
-    <row r="398" ht="12.75" customHeight="1"/>
-    <row r="399" ht="12.75" customHeight="1"/>
-    <row r="400" ht="12.75" customHeight="1"/>
-    <row r="401" ht="12.75" customHeight="1"/>
-    <row r="402" ht="12.75" customHeight="1"/>
-    <row r="403" ht="12.75" customHeight="1"/>
-    <row r="404" ht="12.75" customHeight="1"/>
-    <row r="405" ht="12.75" customHeight="1"/>
-    <row r="406" ht="12.75" customHeight="1"/>
-    <row r="407" ht="12.75" customHeight="1"/>
-    <row r="408" ht="12.75" customHeight="1"/>
-    <row r="409" ht="12.75" customHeight="1"/>
-    <row r="410" ht="12.75" customHeight="1"/>
-    <row r="411" ht="12.75" customHeight="1"/>
-    <row r="412" ht="12.75" customHeight="1"/>
-    <row r="413" ht="12.75" customHeight="1"/>
-    <row r="414" ht="12.75" customHeight="1"/>
-    <row r="415" ht="12.75" customHeight="1"/>
-    <row r="416" ht="12.75" customHeight="1"/>
-    <row r="417" ht="12.75" customHeight="1"/>
-    <row r="418" ht="12.75" customHeight="1"/>
-    <row r="419" ht="12.75" customHeight="1"/>
-    <row r="420" ht="12.75" customHeight="1"/>
-    <row r="421" ht="12.75" customHeight="1"/>
-    <row r="422" ht="12.75" customHeight="1"/>
-    <row r="423" ht="12.75" customHeight="1"/>
-    <row r="424" ht="12.75" customHeight="1"/>
-    <row r="425" ht="12.75" customHeight="1"/>
-    <row r="426" ht="12.75" customHeight="1"/>
-    <row r="427" ht="12.75" customHeight="1"/>
-    <row r="428" ht="12.75" customHeight="1"/>
-    <row r="429" ht="12.75" customHeight="1"/>
-    <row r="430" ht="12.75" customHeight="1"/>
-    <row r="431" ht="12.75" customHeight="1"/>
-    <row r="432" ht="12.75" customHeight="1"/>
-    <row r="433" ht="12.75" customHeight="1"/>
-    <row r="434" ht="12.75" customHeight="1"/>
-    <row r="435" ht="12.75" customHeight="1"/>
-    <row r="436" ht="12.75" customHeight="1"/>
-    <row r="437" ht="12.75" customHeight="1"/>
-    <row r="438" ht="12.75" customHeight="1"/>
-    <row r="439" ht="12.75" customHeight="1"/>
-    <row r="440" ht="12.75" customHeight="1"/>
-    <row r="441" ht="12.75" customHeight="1"/>
-    <row r="442" ht="12.75" customHeight="1"/>
-    <row r="443" ht="12.75" customHeight="1"/>
-    <row r="444" ht="12.75" customHeight="1"/>
-    <row r="445" ht="12.75" customHeight="1"/>
-    <row r="446" ht="12.75" customHeight="1"/>
-    <row r="447" ht="12.75" customHeight="1"/>
-    <row r="448" ht="12.75" customHeight="1"/>
-    <row r="449" ht="12.75" customHeight="1"/>
-    <row r="450" ht="12.75" customHeight="1"/>
-    <row r="451" ht="12.75" customHeight="1"/>
-    <row r="452" ht="12.75" customHeight="1"/>
-    <row r="453" ht="12.75" customHeight="1"/>
-    <row r="454" ht="12.75" customHeight="1"/>
-    <row r="455" ht="12.75" customHeight="1"/>
-    <row r="456" ht="12.75" customHeight="1"/>
-    <row r="457" ht="12.75" customHeight="1"/>
-    <row r="458" ht="12.75" customHeight="1"/>
-    <row r="459" ht="12.75" customHeight="1"/>
-    <row r="460" ht="12.75" customHeight="1"/>
-    <row r="461" ht="12.75" customHeight="1"/>
-    <row r="462" ht="12.75" customHeight="1"/>
-    <row r="463" ht="12.75" customHeight="1"/>
-    <row r="464" ht="12.75" customHeight="1"/>
-    <row r="465" ht="12.75" customHeight="1"/>
-    <row r="466" ht="12.75" customHeight="1"/>
-    <row r="467" ht="12.75" customHeight="1"/>
-    <row r="468" ht="12.75" customHeight="1"/>
-    <row r="469" ht="12.75" customHeight="1"/>
-    <row r="470" ht="12.75" customHeight="1"/>
-    <row r="471" ht="12.75" customHeight="1"/>
-    <row r="472" ht="12.75" customHeight="1"/>
-    <row r="473" ht="12.75" customHeight="1"/>
-    <row r="474" ht="12.75" customHeight="1"/>
-    <row r="475" ht="12.75" customHeight="1"/>
-    <row r="476" ht="12.75" customHeight="1"/>
-    <row r="477" ht="12.75" customHeight="1"/>
-    <row r="478" ht="12.75" customHeight="1"/>
-    <row r="479" ht="12.75" customHeight="1"/>
-    <row r="480" ht="12.75" customHeight="1"/>
-    <row r="481" ht="12.75" customHeight="1"/>
-    <row r="482" ht="12.75" customHeight="1"/>
-    <row r="483" ht="12.75" customHeight="1"/>
-    <row r="484" ht="12.75" customHeight="1"/>
-    <row r="485" ht="12.75" customHeight="1"/>
-    <row r="486" ht="12.75" customHeight="1"/>
-    <row r="487" ht="12.75" customHeight="1"/>
-    <row r="488" ht="12.75" customHeight="1"/>
-    <row r="489" ht="12.75" customHeight="1"/>
-    <row r="490" ht="12.75" customHeight="1"/>
-    <row r="491" ht="12.75" customHeight="1"/>
-    <row r="492" ht="12.75" customHeight="1"/>
-    <row r="493" ht="12.75" customHeight="1"/>
-    <row r="494" ht="12.75" customHeight="1"/>
-    <row r="495" ht="12.75" customHeight="1"/>
-    <row r="496" ht="12.75" customHeight="1"/>
-    <row r="497" ht="12.75" customHeight="1"/>
-    <row r="498" ht="12.75" customHeight="1"/>
-    <row r="499" ht="12.75" customHeight="1"/>
-    <row r="500" ht="12.75" customHeight="1"/>
-    <row r="501" ht="12.75" customHeight="1"/>
-    <row r="502" ht="12.75" customHeight="1"/>
-    <row r="503" ht="12.75" customHeight="1"/>
-    <row r="504" ht="12.75" customHeight="1"/>
-    <row r="505" ht="12.75" customHeight="1"/>
-    <row r="506" ht="12.75" customHeight="1"/>
-    <row r="507" ht="12.75" customHeight="1"/>
-    <row r="508" ht="12.75" customHeight="1"/>
-    <row r="509" ht="12.75" customHeight="1"/>
-    <row r="510" ht="12.75" customHeight="1"/>
-    <row r="511" ht="12.75" customHeight="1"/>
-    <row r="512" ht="12.75" customHeight="1"/>
-    <row r="513" ht="12.75" customHeight="1"/>
-    <row r="514" ht="12.75" customHeight="1"/>
-    <row r="515" ht="12.75" customHeight="1"/>
-    <row r="516" ht="12.75" customHeight="1"/>
-    <row r="517" ht="12.75" customHeight="1"/>
-    <row r="518" ht="12.75" customHeight="1"/>
-    <row r="519" ht="12.75" customHeight="1"/>
-    <row r="520" ht="12.75" customHeight="1"/>
-    <row r="521" ht="12.75" customHeight="1"/>
-    <row r="522" ht="12.75" customHeight="1"/>
-    <row r="523" ht="12.75" customHeight="1"/>
-    <row r="524" ht="12.75" customHeight="1"/>
-    <row r="525" ht="12.75" customHeight="1"/>
-    <row r="526" ht="12.75" customHeight="1"/>
-    <row r="527" ht="12.75" customHeight="1"/>
-    <row r="528" ht="12.75" customHeight="1"/>
-    <row r="529" ht="12.75" customHeight="1"/>
-    <row r="530" ht="12.75" customHeight="1"/>
-    <row r="531" ht="12.75" customHeight="1"/>
-    <row r="532" ht="12.75" customHeight="1"/>
-    <row r="533" ht="12.75" customHeight="1"/>
-    <row r="534" ht="12.75" customHeight="1"/>
-    <row r="535" ht="12.75" customHeight="1"/>
-    <row r="536" ht="12.75" customHeight="1"/>
-    <row r="537" ht="12.75" customHeight="1"/>
-    <row r="538" ht="12.75" customHeight="1"/>
-    <row r="539" ht="12.75" customHeight="1"/>
-    <row r="540" ht="12.75" customHeight="1"/>
-    <row r="541" ht="12.75" customHeight="1"/>
-    <row r="542" ht="12.75" customHeight="1"/>
-    <row r="543" ht="12.75" customHeight="1"/>
-    <row r="544" ht="12.75" customHeight="1"/>
-    <row r="545" ht="12.75" customHeight="1"/>
-    <row r="546" ht="12.75" customHeight="1"/>
-    <row r="547" ht="12.75" customHeight="1"/>
-    <row r="548" ht="12.75" customHeight="1"/>
-    <row r="549" ht="12.75" customHeight="1"/>
-    <row r="550" ht="12.75" customHeight="1"/>
-    <row r="551" ht="12.75" customHeight="1"/>
-    <row r="552" ht="12.75" customHeight="1"/>
-    <row r="553" ht="12.75" customHeight="1"/>
-    <row r="554" ht="12.75" customHeight="1"/>
-    <row r="555" ht="12.75" customHeight="1"/>
-    <row r="556" ht="12.75" customHeight="1"/>
-    <row r="557" ht="12.75" customHeight="1"/>
-    <row r="558" ht="12.75" customHeight="1"/>
-    <row r="559" ht="12.75" customHeight="1"/>
-    <row r="560" ht="12.75" customHeight="1"/>
-    <row r="561" ht="12.75" customHeight="1"/>
-    <row r="562" ht="12.75" customHeight="1"/>
-    <row r="563" ht="12.75" customHeight="1"/>
-    <row r="564" ht="12.75" customHeight="1"/>
-    <row r="565" ht="12.75" customHeight="1"/>
-    <row r="566" ht="12.75" customHeight="1"/>
-    <row r="567" ht="12.75" customHeight="1"/>
-    <row r="568" ht="12.75" customHeight="1"/>
-    <row r="569" ht="12.75" customHeight="1"/>
-    <row r="570" ht="12.75" customHeight="1"/>
-    <row r="571" ht="12.75" customHeight="1"/>
-    <row r="572" ht="12.75" customHeight="1"/>
-    <row r="573" ht="12.75" customHeight="1"/>
-    <row r="574" ht="12.75" customHeight="1"/>
-    <row r="575" ht="12.75" customHeight="1"/>
-    <row r="576" ht="12.75" customHeight="1"/>
-    <row r="577" ht="12.75" customHeight="1"/>
-    <row r="578" ht="12.75" customHeight="1"/>
-    <row r="579" ht="12.75" customHeight="1"/>
-    <row r="580" ht="12.75" customHeight="1"/>
-    <row r="581" ht="12.75" customHeight="1"/>
-    <row r="582" ht="12.75" customHeight="1"/>
-    <row r="583" ht="12.75" customHeight="1"/>
-    <row r="584" ht="12.75" customHeight="1"/>
-    <row r="585" ht="12.75" customHeight="1"/>
-    <row r="586" ht="12.75" customHeight="1"/>
-    <row r="587" ht="12.75" customHeight="1"/>
-    <row r="588" ht="12.75" customHeight="1"/>
-    <row r="589" ht="12.75" customHeight="1"/>
-    <row r="590" ht="12.75" customHeight="1"/>
-    <row r="591" ht="12.75" customHeight="1"/>
-    <row r="592" ht="12.75" customHeight="1"/>
-    <row r="593" ht="12.75" customHeight="1"/>
-    <row r="594" ht="12.75" customHeight="1"/>
-    <row r="595" ht="12.75" customHeight="1"/>
-    <row r="596" ht="12.75" customHeight="1"/>
-    <row r="597" ht="12.75" customHeight="1"/>
-    <row r="598" ht="12.75" customHeight="1"/>
-    <row r="599" ht="12.75" customHeight="1"/>
-    <row r="600" ht="12.75" customHeight="1"/>
-    <row r="601" ht="12.75" customHeight="1"/>
-    <row r="602" ht="12.75" customHeight="1"/>
-    <row r="603" ht="12.75" customHeight="1"/>
-    <row r="604" ht="12.75" customHeight="1"/>
-    <row r="605" ht="12.75" customHeight="1"/>
-    <row r="606" ht="12.75" customHeight="1"/>
-    <row r="607" ht="12.75" customHeight="1"/>
-    <row r="608" ht="12.75" customHeight="1"/>
-    <row r="609" ht="12.75" customHeight="1"/>
-    <row r="610" ht="12.75" customHeight="1"/>
-    <row r="611" ht="12.75" customHeight="1"/>
-    <row r="612" ht="12.75" customHeight="1"/>
-    <row r="613" ht="12.75" customHeight="1"/>
-    <row r="614" ht="12.75" customHeight="1"/>
-    <row r="615" ht="12.75" customHeight="1"/>
-    <row r="616" ht="12.75" customHeight="1"/>
-    <row r="617" ht="12.75" customHeight="1"/>
-    <row r="618" ht="12.75" customHeight="1"/>
-    <row r="619" ht="12.75" customHeight="1"/>
-    <row r="620" ht="12.75" customHeight="1"/>
-    <row r="621" ht="12.75" customHeight="1"/>
-    <row r="622" ht="12.75" customHeight="1"/>
-    <row r="623" ht="12.75" customHeight="1"/>
-    <row r="624" ht="12.75" customHeight="1"/>
-    <row r="625" ht="12.75" customHeight="1"/>
-    <row r="626" ht="12.75" customHeight="1"/>
-    <row r="627" ht="12.75" customHeight="1"/>
-    <row r="628" ht="12.75" customHeight="1"/>
-    <row r="629" ht="12.75" customHeight="1"/>
-    <row r="630" ht="12.75" customHeight="1"/>
-    <row r="631" ht="12.75" customHeight="1"/>
-    <row r="632" ht="12.75" customHeight="1"/>
-    <row r="633" ht="12.75" customHeight="1"/>
-    <row r="634" ht="12.75" customHeight="1"/>
-    <row r="635" ht="12.75" customHeight="1"/>
-    <row r="636" ht="12.75" customHeight="1"/>
-    <row r="637" ht="12.75" customHeight="1"/>
-    <row r="638" ht="12.75" customHeight="1"/>
-    <row r="639" ht="12.75" customHeight="1"/>
-    <row r="640" ht="12.75" customHeight="1"/>
-    <row r="641" ht="12.75" customHeight="1"/>
-    <row r="642" ht="12.75" customHeight="1"/>
-    <row r="643" ht="12.75" customHeight="1"/>
-    <row r="644" ht="12.75" customHeight="1"/>
-    <row r="645" ht="12.75" customHeight="1"/>
-    <row r="646" ht="12.75" customHeight="1"/>
-    <row r="647" ht="12.75" customHeight="1"/>
-    <row r="648" ht="12.75" customHeight="1"/>
-    <row r="649" ht="12.75" customHeight="1"/>
-    <row r="650" ht="12.75" customHeight="1"/>
-    <row r="651" ht="12.75" customHeight="1"/>
-    <row r="652" ht="12.75" customHeight="1"/>
-    <row r="653" ht="12.75" customHeight="1"/>
-    <row r="654" ht="12.75" customHeight="1"/>
-    <row r="655" ht="12.75" customHeight="1"/>
-    <row r="656" ht="12.75" customHeight="1"/>
-    <row r="657" ht="12.75" customHeight="1"/>
-    <row r="658" ht="12.75" customHeight="1"/>
-    <row r="659" ht="12.75" customHeight="1"/>
-    <row r="660" ht="12.75" customHeight="1"/>
-    <row r="661" ht="12.75" customHeight="1"/>
-    <row r="662" ht="12.75" customHeight="1"/>
-    <row r="663" ht="12.75" customHeight="1"/>
-    <row r="664" ht="12.75" customHeight="1"/>
-    <row r="665" ht="12.75" customHeight="1"/>
-    <row r="666" ht="12.75" customHeight="1"/>
-    <row r="667" ht="12.75" customHeight="1"/>
-    <row r="668" ht="12.75" customHeight="1"/>
-    <row r="669" ht="12.75" customHeight="1"/>
-    <row r="670" ht="12.75" customHeight="1"/>
-    <row r="671" ht="12.75" customHeight="1"/>
-    <row r="672" ht="12.75" customHeight="1"/>
-    <row r="673" ht="12.75" customHeight="1"/>
-    <row r="674" ht="12.75" customHeight="1"/>
-    <row r="675" ht="12.75" customHeight="1"/>
-    <row r="676" ht="12.75" customHeight="1"/>
-    <row r="677" ht="12.75" customHeight="1"/>
-    <row r="678" ht="12.75" customHeight="1"/>
-    <row r="679" ht="12.75" customHeight="1"/>
-    <row r="680" ht="12.75" customHeight="1"/>
-    <row r="681" ht="12.75" customHeight="1"/>
-    <row r="682" ht="12.75" customHeight="1"/>
-    <row r="683" ht="12.75" customHeight="1"/>
-    <row r="684" ht="12.75" customHeight="1"/>
-    <row r="685" ht="12.75" customHeight="1"/>
-    <row r="686" ht="12.75" customHeight="1"/>
-    <row r="687" ht="12.75" customHeight="1"/>
-    <row r="688" ht="12.75" customHeight="1"/>
-    <row r="689" ht="12.75" customHeight="1"/>
-    <row r="690" ht="12.75" customHeight="1"/>
-    <row r="691" ht="12.75" customHeight="1"/>
-    <row r="692" ht="12.75" customHeight="1"/>
-    <row r="693" ht="12.75" customHeight="1"/>
-    <row r="694" ht="12.75" customHeight="1"/>
-    <row r="695" ht="12.75" customHeight="1"/>
-    <row r="696" ht="12.75" customHeight="1"/>
-    <row r="697" ht="12.75" customHeight="1"/>
-    <row r="698" ht="12.75" customHeight="1"/>
-    <row r="699" ht="12.75" customHeight="1"/>
-    <row r="700" ht="12.75" customHeight="1"/>
-    <row r="701" ht="12.75" customHeight="1"/>
-    <row r="702" ht="12.75" customHeight="1"/>
-    <row r="703" ht="12.75" customHeight="1"/>
-    <row r="704" ht="12.75" customHeight="1"/>
-    <row r="705" ht="12.75" customHeight="1"/>
-    <row r="706" ht="12.75" customHeight="1"/>
-    <row r="707" ht="12.75" customHeight="1"/>
-    <row r="708" ht="12.75" customHeight="1"/>
-    <row r="709" ht="12.75" customHeight="1"/>
-    <row r="710" ht="12.75" customHeight="1"/>
-    <row r="711" ht="12.75" customHeight="1"/>
-    <row r="712" ht="12.75" customHeight="1"/>
-    <row r="713" ht="12.75" customHeight="1"/>
-    <row r="714" ht="12.75" customHeight="1"/>
-    <row r="715" ht="12.75" customHeight="1"/>
-    <row r="716" ht="12.75" customHeight="1"/>
-    <row r="717" ht="12.75" customHeight="1"/>
-    <row r="718" ht="12.75" customHeight="1"/>
-    <row r="719" ht="12.75" customHeight="1"/>
-    <row r="720" ht="12.75" customHeight="1"/>
-    <row r="721" ht="12.75" customHeight="1"/>
-    <row r="722" ht="12.75" customHeight="1"/>
-    <row r="723" ht="12.75" customHeight="1"/>
-    <row r="724" ht="12.75" customHeight="1"/>
-    <row r="725" ht="12.75" customHeight="1"/>
-    <row r="726" ht="12.75" customHeight="1"/>
-    <row r="727" ht="12.75" customHeight="1"/>
-    <row r="728" ht="12.75" customHeight="1"/>
-    <row r="729" ht="12.75" customHeight="1"/>
-    <row r="730" ht="12.75" customHeight="1"/>
-    <row r="731" ht="12.75" customHeight="1"/>
-    <row r="732" ht="12.75" customHeight="1"/>
-    <row r="733" ht="12.75" customHeight="1"/>
-    <row r="734" ht="12.75" customHeight="1"/>
-    <row r="735" ht="12.75" customHeight="1"/>
-    <row r="736" ht="12.75" customHeight="1"/>
-    <row r="737" ht="12.75" customHeight="1"/>
-    <row r="738" ht="12.75" customHeight="1"/>
-    <row r="739" ht="12.75" customHeight="1"/>
-    <row r="740" ht="12.75" customHeight="1"/>
-    <row r="741" ht="12.75" customHeight="1"/>
-    <row r="742" ht="12.75" customHeight="1"/>
-    <row r="743" ht="12.75" customHeight="1"/>
-    <row r="744" ht="12.75" customHeight="1"/>
-    <row r="745" ht="12.75" customHeight="1"/>
-    <row r="746" ht="12.75" customHeight="1"/>
-    <row r="747" ht="12.75" customHeight="1"/>
-    <row r="748" ht="12.75" customHeight="1"/>
-    <row r="749" ht="12.75" customHeight="1"/>
-    <row r="750" ht="12.75" customHeight="1"/>
-    <row r="751" ht="12.75" customHeight="1"/>
-    <row r="752" ht="12.75" customHeight="1"/>
-    <row r="753" ht="12.75" customHeight="1"/>
-    <row r="754" ht="12.75" customHeight="1"/>
-    <row r="755" ht="12.75" customHeight="1"/>
-    <row r="756" ht="12.75" customHeight="1"/>
-    <row r="757" ht="12.75" customHeight="1"/>
-    <row r="758" ht="12.75" customHeight="1"/>
-    <row r="759" ht="12.75" customHeight="1"/>
-    <row r="760" ht="12.75" customHeight="1"/>
-    <row r="761" ht="12.75" customHeight="1"/>
-    <row r="762" ht="12.75" customHeight="1"/>
-    <row r="763" ht="12.75" customHeight="1"/>
-    <row r="764" ht="12.75" customHeight="1"/>
-    <row r="765" ht="12.75" customHeight="1"/>
-    <row r="766" ht="12.75" customHeight="1"/>
-    <row r="767" ht="12.75" customHeight="1"/>
-    <row r="768" ht="12.75" customHeight="1"/>
-    <row r="769" ht="12.75" customHeight="1"/>
-    <row r="770" ht="12.75" customHeight="1"/>
-    <row r="771" ht="12.75" customHeight="1"/>
-    <row r="772" ht="12.75" customHeight="1"/>
-    <row r="773" ht="12.75" customHeight="1"/>
-    <row r="774" ht="12.75" customHeight="1"/>
-    <row r="775" ht="12.75" customHeight="1"/>
-    <row r="776" ht="12.75" customHeight="1"/>
-    <row r="777" ht="12.75" customHeight="1"/>
-    <row r="778" ht="12.75" customHeight="1"/>
-    <row r="779" ht="12.75" customHeight="1"/>
-    <row r="780" ht="12.75" customHeight="1"/>
-    <row r="781" ht="12.75" customHeight="1"/>
-    <row r="782" ht="12.75" customHeight="1"/>
-    <row r="783" ht="12.75" customHeight="1"/>
-    <row r="784" ht="12.75" customHeight="1"/>
-    <row r="785" ht="12.75" customHeight="1"/>
-    <row r="786" ht="12.75" customHeight="1"/>
-    <row r="787" ht="12.75" customHeight="1"/>
-    <row r="788" ht="12.75" customHeight="1"/>
-    <row r="789" ht="12.75" customHeight="1"/>
-    <row r="790" ht="12.75" customHeight="1"/>
-    <row r="791" ht="12.75" customHeight="1"/>
-    <row r="792" ht="12.75" customHeight="1"/>
-    <row r="793" ht="12.75" customHeight="1"/>
-    <row r="794" ht="12.75" customHeight="1"/>
-    <row r="795" ht="12.75" customHeight="1"/>
-    <row r="796" ht="12.75" customHeight="1"/>
-    <row r="797" ht="12.75" customHeight="1"/>
-    <row r="798" ht="12.75" customHeight="1"/>
-    <row r="799" ht="12.75" customHeight="1"/>
-    <row r="800" ht="12.75" customHeight="1"/>
-    <row r="801" ht="12.75" customHeight="1"/>
-    <row r="802" ht="12.75" customHeight="1"/>
-    <row r="803" ht="12.75" customHeight="1"/>
-    <row r="804" ht="12.75" customHeight="1"/>
-    <row r="805" ht="12.75" customHeight="1"/>
-    <row r="806" ht="12.75" customHeight="1"/>
-    <row r="807" ht="12.75" customHeight="1"/>
-    <row r="808" ht="12.75" customHeight="1"/>
-    <row r="809" ht="12.75" customHeight="1"/>
-    <row r="810" ht="12.75" customHeight="1"/>
-    <row r="811" ht="12.75" customHeight="1"/>
-    <row r="812" ht="12.75" customHeight="1"/>
-    <row r="813" ht="12.75" customHeight="1"/>
-    <row r="814" ht="12.75" customHeight="1"/>
-    <row r="815" ht="12.75" customHeight="1"/>
-    <row r="816" ht="12.75" customHeight="1"/>
-    <row r="817" ht="12.75" customHeight="1"/>
-    <row r="818" ht="12.75" customHeight="1"/>
-    <row r="819" ht="12.75" customHeight="1"/>
-    <row r="820" ht="12.75" customHeight="1"/>
-    <row r="821" ht="12.75" customHeight="1"/>
-    <row r="822" ht="12.75" customHeight="1"/>
-    <row r="823" ht="12.75" customHeight="1"/>
-    <row r="824" ht="12.75" customHeight="1"/>
-    <row r="825" ht="12.75" customHeight="1"/>
-    <row r="826" ht="12.75" customHeight="1"/>
-    <row r="827" ht="12.75" customHeight="1"/>
-    <row r="828" ht="12.75" customHeight="1"/>
-    <row r="829" ht="12.75" customHeight="1"/>
-    <row r="830" ht="12.75" customHeight="1"/>
-    <row r="831" ht="12.75" customHeight="1"/>
-    <row r="832" ht="12.75" customHeight="1"/>
-    <row r="833" ht="12.75" customHeight="1"/>
-    <row r="834" ht="12.75" customHeight="1"/>
-    <row r="835" ht="12.75" customHeight="1"/>
-    <row r="836" ht="12.75" customHeight="1"/>
-    <row r="837" ht="12.75" customHeight="1"/>
-    <row r="838" ht="12.75" customHeight="1"/>
-    <row r="839" ht="12.75" customHeight="1"/>
-    <row r="840" ht="12.75" customHeight="1"/>
-    <row r="841" ht="12.75" customHeight="1"/>
-    <row r="842" ht="12.75" customHeight="1"/>
-    <row r="843" ht="12.75" customHeight="1"/>
-    <row r="844" ht="12.75" customHeight="1"/>
-    <row r="845" ht="12.75" customHeight="1"/>
-    <row r="846" ht="12.75" customHeight="1"/>
-    <row r="847" ht="12.75" customHeight="1"/>
-    <row r="848" ht="12.75" customHeight="1"/>
-    <row r="849" ht="12.75" customHeight="1"/>
-    <row r="850" ht="12.75" customHeight="1"/>
-    <row r="851" ht="12.75" customHeight="1"/>
-    <row r="852" ht="12.75" customHeight="1"/>
-    <row r="853" ht="12.75" customHeight="1"/>
-    <row r="854" ht="12.75" customHeight="1"/>
-    <row r="855" ht="12.75" customHeight="1"/>
-    <row r="856" ht="12.75" customHeight="1"/>
-    <row r="857" ht="12.75" customHeight="1"/>
-    <row r="858" ht="12.75" customHeight="1"/>
-    <row r="859" ht="12.75" customHeight="1"/>
-    <row r="860" ht="12.75" customHeight="1"/>
-    <row r="861" ht="12.75" customHeight="1"/>
-    <row r="862" ht="12.75" customHeight="1"/>
-    <row r="863" ht="12.75" customHeight="1"/>
-    <row r="864" ht="12.75" customHeight="1"/>
-    <row r="865" ht="12.75" customHeight="1"/>
-    <row r="866" ht="12.75" customHeight="1"/>
-    <row r="867" ht="12.75" customHeight="1"/>
-    <row r="868" ht="12.75" customHeight="1"/>
-    <row r="869" ht="12.75" customHeight="1"/>
-    <row r="870" ht="12.75" customHeight="1"/>
-    <row r="871" ht="12.75" customHeight="1"/>
-    <row r="872" ht="12.75" customHeight="1"/>
-    <row r="873" ht="12.75" customHeight="1"/>
-    <row r="874" ht="12.75" customHeight="1"/>
-    <row r="875" ht="12.75" customHeight="1"/>
-    <row r="876" ht="12.75" customHeight="1"/>
-    <row r="877" ht="12.75" customHeight="1"/>
-    <row r="878" ht="12.75" customHeight="1"/>
-    <row r="879" ht="12.75" customHeight="1"/>
-    <row r="880" ht="12.75" customHeight="1"/>
-    <row r="881" ht="12.75" customHeight="1"/>
-    <row r="882" ht="12.75" customHeight="1"/>
-    <row r="883" ht="12.75" customHeight="1"/>
-    <row r="884" ht="12.75" customHeight="1"/>
-    <row r="885" ht="12.75" customHeight="1"/>
-    <row r="886" ht="12.75" customHeight="1"/>
-    <row r="887" ht="12.75" customHeight="1"/>
-    <row r="888" ht="12.75" customHeight="1"/>
-    <row r="889" ht="12.75" customHeight="1"/>
-    <row r="890" ht="12.75" customHeight="1"/>
-    <row r="891" ht="12.75" customHeight="1"/>
-    <row r="892" ht="12.75" customHeight="1"/>
-    <row r="893" ht="12.75" customHeight="1"/>
-    <row r="894" ht="12.75" customHeight="1"/>
-    <row r="895" ht="12.75" customHeight="1"/>
-    <row r="896" ht="12.75" customHeight="1"/>
-    <row r="897" ht="12.75" customHeight="1"/>
-    <row r="898" ht="12.75" customHeight="1"/>
-    <row r="899" ht="12.75" customHeight="1"/>
-    <row r="900" ht="12.75" customHeight="1"/>
-    <row r="901" ht="12.75" customHeight="1"/>
-    <row r="902" ht="12.75" customHeight="1"/>
-    <row r="903" ht="12.75" customHeight="1"/>
-    <row r="904" ht="12.75" customHeight="1"/>
-    <row r="905" ht="12.75" customHeight="1"/>
-    <row r="906" ht="12.75" customHeight="1"/>
-    <row r="907" ht="12.75" customHeight="1"/>
-    <row r="908" ht="12.75" customHeight="1"/>
-    <row r="909" ht="12.75" customHeight="1"/>
-    <row r="910" ht="12.75" customHeight="1"/>
-    <row r="911" ht="12.75" customHeight="1"/>
-    <row r="912" ht="12.75" customHeight="1"/>
-    <row r="913" ht="12.75" customHeight="1"/>
-    <row r="914" ht="12.75" customHeight="1"/>
-    <row r="915" ht="12.75" customHeight="1"/>
-    <row r="916" ht="12.75" customHeight="1"/>
-    <row r="917" ht="12.75" customHeight="1"/>
-    <row r="918" ht="12.75" customHeight="1"/>
-    <row r="919" ht="12.75" customHeight="1"/>
-    <row r="920" ht="12.75" customHeight="1"/>
-    <row r="921" ht="12.75" customHeight="1"/>
-    <row r="922" ht="12.75" customHeight="1"/>
-    <row r="923" ht="12.75" customHeight="1"/>
-    <row r="924" ht="12.75" customHeight="1"/>
-    <row r="925" ht="12.75" customHeight="1"/>
-    <row r="926" ht="12.75" customHeight="1"/>
-    <row r="927" ht="12.75" customHeight="1"/>
-    <row r="928" ht="12.75" customHeight="1"/>
-    <row r="929" ht="12.75" customHeight="1"/>
-    <row r="930" ht="12.75" customHeight="1"/>
-    <row r="931" ht="12.75" customHeight="1"/>
-    <row r="932" ht="12.75" customHeight="1"/>
-    <row r="933" ht="12.75" customHeight="1"/>
-    <row r="934" ht="12.75" customHeight="1"/>
-    <row r="935" ht="12.75" customHeight="1"/>
-    <row r="936" ht="12.75" customHeight="1"/>
-    <row r="937" ht="12.75" customHeight="1"/>
-    <row r="938" ht="12.75" customHeight="1"/>
-    <row r="939" ht="12.75" customHeight="1"/>
-    <row r="940" ht="12.75" customHeight="1"/>
-    <row r="941" ht="12.75" customHeight="1"/>
-    <row r="942" ht="12.75" customHeight="1"/>
-    <row r="943" ht="12.75" customHeight="1"/>
-    <row r="944" ht="12.75" customHeight="1"/>
-    <row r="945" ht="12.75" customHeight="1"/>
-    <row r="946" ht="12.75" customHeight="1"/>
-    <row r="947" ht="12.75" customHeight="1"/>
-    <row r="948" ht="12.75" customHeight="1"/>
-    <row r="949" ht="12.75" customHeight="1"/>
-    <row r="950" ht="12.75" customHeight="1"/>
-    <row r="951" ht="12.75" customHeight="1"/>
-    <row r="952" ht="12.75" customHeight="1"/>
-    <row r="953" ht="12.75" customHeight="1"/>
-    <row r="954" ht="12.75" customHeight="1"/>
-    <row r="955" ht="12.75" customHeight="1"/>
-    <row r="956" ht="12.75" customHeight="1"/>
-    <row r="957" ht="12.75" customHeight="1"/>
-    <row r="958" ht="12.75" customHeight="1"/>
-    <row r="959" ht="12.75" customHeight="1"/>
-    <row r="960" ht="12.75" customHeight="1"/>
-    <row r="961" ht="12.75" customHeight="1"/>
-    <row r="962" ht="12.75" customHeight="1"/>
-    <row r="963" ht="12.75" customHeight="1"/>
-    <row r="964" ht="12.75" customHeight="1"/>
-    <row r="965" ht="12.75" customHeight="1"/>
-    <row r="966" ht="12.75" customHeight="1"/>
-    <row r="967" ht="12.75" customHeight="1"/>
-    <row r="968" ht="12.75" customHeight="1"/>
-    <row r="969" ht="12.75" customHeight="1"/>
-    <row r="970" ht="12.75" customHeight="1"/>
-    <row r="971" ht="12.75" customHeight="1"/>
-    <row r="972" ht="12.75" customHeight="1"/>
-    <row r="973" ht="12.75" customHeight="1"/>
-    <row r="974" ht="12.75" customHeight="1"/>
-    <row r="975" ht="12.75" customHeight="1"/>
-    <row r="976" ht="12.75" customHeight="1"/>
-    <row r="977" ht="12.75" customHeight="1"/>
-    <row r="978" ht="12.75" customHeight="1"/>
-    <row r="979" ht="12.75" customHeight="1"/>
-    <row r="980" ht="12.75" customHeight="1"/>
-    <row r="981" ht="12.75" customHeight="1"/>
-    <row r="982" ht="12.75" customHeight="1"/>
-    <row r="983" ht="12.75" customHeight="1"/>
-    <row r="984" ht="12.75" customHeight="1"/>
-    <row r="985" ht="12.75" customHeight="1"/>
-    <row r="986" ht="12.75" customHeight="1"/>
-    <row r="987" ht="12.75" customHeight="1"/>
-    <row r="988" ht="12.75" customHeight="1"/>
-    <row r="989" ht="12.75" customHeight="1"/>
-    <row r="990" ht="12.75" customHeight="1"/>
-    <row r="991" ht="12.75" customHeight="1"/>
-    <row r="992" ht="12.75" customHeight="1"/>
-    <row r="993" ht="12.75" customHeight="1"/>
-    <row r="994" ht="12.75" customHeight="1"/>
-    <row r="995" ht="12.75" customHeight="1"/>
-    <row r="996" ht="12.75" customHeight="1"/>
-    <row r="997" ht="12.75" customHeight="1"/>
-    <row r="998" ht="12.75" customHeight="1"/>
-    <row r="999" ht="12.75" customHeight="1"/>
-    <row r="1000" ht="12.75" customHeight="1"/>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins bottom="0.3" footer="0.0" header="0.0" left="0.3" right="0.3" top="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="26" width="0.71"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="12.75" customHeight="1"/>
-    <row r="2" ht="12.75" customHeight="1"/>
-    <row r="3" ht="12.75" customHeight="1"/>
-    <row r="4" ht="12.75" customHeight="1"/>
-    <row r="5" ht="12.75" customHeight="1"/>
-    <row r="6" ht="12.75" customHeight="1"/>
-    <row r="7" ht="12.75" customHeight="1"/>
-    <row r="8" ht="12.75" customHeight="1"/>
-    <row r="9" ht="12.75" customHeight="1"/>
-    <row r="10" ht="12.75" customHeight="1"/>
-    <row r="11" ht="12.75" customHeight="1"/>
-    <row r="12" ht="12.75" customHeight="1"/>
-    <row r="13" ht="12.75" customHeight="1"/>
-    <row r="14" ht="12.75" customHeight="1"/>
-    <row r="15" ht="12.75" customHeight="1"/>
-    <row r="16" ht="12.75" customHeight="1"/>
-    <row r="17" ht="12.75" customHeight="1"/>
-    <row r="18" ht="12.75" customHeight="1"/>
-    <row r="19" ht="12.75" customHeight="1"/>
-    <row r="20" ht="12.75" customHeight="1"/>
-    <row r="21" ht="12.75" customHeight="1"/>
-    <row r="22" ht="12.75" customHeight="1"/>
-    <row r="23" ht="12.75" customHeight="1"/>
-    <row r="24" ht="12.75" customHeight="1"/>
-    <row r="25" ht="12.75" customHeight="1"/>
-    <row r="26" ht="12.75" customHeight="1"/>
-    <row r="27" ht="12.75" customHeight="1"/>
-    <row r="28" ht="12.75" customHeight="1"/>
-    <row r="29" ht="12.75" customHeight="1"/>
-    <row r="30" ht="12.75" customHeight="1"/>
-    <row r="31" ht="12.75" customHeight="1"/>
-    <row r="32" ht="12.75" customHeight="1"/>
-    <row r="33" ht="12.75" customHeight="1"/>
-    <row r="34" ht="12.75" customHeight="1"/>
-    <row r="35" ht="12.75" customHeight="1"/>
-    <row r="36" ht="12.75" customHeight="1"/>
-    <row r="37" ht="12.75" customHeight="1"/>
-    <row r="38" ht="12.75" customHeight="1"/>
-    <row r="39" ht="12.75" customHeight="1"/>
-    <row r="40" ht="12.75" customHeight="1"/>
-    <row r="41" ht="12.75" customHeight="1"/>
-    <row r="42" ht="12.75" customHeight="1"/>
-    <row r="43" ht="12.75" customHeight="1"/>
-    <row r="44" ht="12.75" customHeight="1"/>
-    <row r="45" ht="12.75" customHeight="1"/>
-    <row r="46" ht="12.75" customHeight="1"/>
-    <row r="47" ht="12.75" customHeight="1"/>
-    <row r="48" ht="12.75" customHeight="1"/>
-    <row r="49" ht="12.75" customHeight="1"/>
-    <row r="50" ht="12.75" customHeight="1"/>
-    <row r="51" ht="12.75" customHeight="1"/>
-    <row r="52" ht="12.75" customHeight="1"/>
-    <row r="53" ht="12.75" customHeight="1"/>
-    <row r="54" ht="12.75" customHeight="1"/>
-    <row r="55" ht="12.75" customHeight="1"/>
-    <row r="56" ht="12.75" customHeight="1"/>
-    <row r="57" ht="12.75" customHeight="1"/>
-    <row r="58" ht="12.75" customHeight="1"/>
-    <row r="59" ht="12.75" customHeight="1"/>
-    <row r="60" ht="12.75" customHeight="1"/>
-    <row r="61" ht="12.75" customHeight="1"/>
-    <row r="62" ht="12.75" customHeight="1"/>
-    <row r="63" ht="12.75" customHeight="1"/>
-    <row r="64" ht="12.75" customHeight="1"/>
-    <row r="65" ht="12.75" customHeight="1"/>
-    <row r="66" ht="12.75" customHeight="1"/>
-    <row r="67" ht="12.75" customHeight="1"/>
-    <row r="68" ht="12.75" customHeight="1"/>
-    <row r="69" ht="12.75" customHeight="1"/>
-    <row r="70" ht="12.75" customHeight="1"/>
-    <row r="71" ht="12.75" customHeight="1"/>
-    <row r="72" ht="12.75" customHeight="1"/>
-    <row r="73" ht="12.75" customHeight="1"/>
-    <row r="74" ht="12.75" customHeight="1"/>
-    <row r="75" ht="12.75" customHeight="1"/>
-    <row r="76" ht="12.75" customHeight="1"/>
-    <row r="77" ht="12.75" customHeight="1"/>
-    <row r="78" ht="12.75" customHeight="1"/>
-    <row r="79" ht="12.75" customHeight="1"/>
-    <row r="80" ht="12.75" customHeight="1"/>
-    <row r="81" ht="12.75" customHeight="1"/>
-    <row r="82" ht="12.75" customHeight="1"/>
-    <row r="83" ht="12.75" customHeight="1"/>
-    <row r="84" ht="12.75" customHeight="1"/>
-    <row r="85" ht="12.75" customHeight="1"/>
-    <row r="86" ht="12.75" customHeight="1"/>
-    <row r="87" ht="12.75" customHeight="1"/>
-    <row r="88" ht="12.75" customHeight="1"/>
-    <row r="89" ht="12.75" customHeight="1"/>
-    <row r="90" ht="12.75" customHeight="1"/>
-    <row r="91" ht="12.75" customHeight="1"/>
-    <row r="92" ht="12.75" customHeight="1"/>
-    <row r="93" ht="12.75" customHeight="1"/>
-    <row r="94" ht="12.75" customHeight="1"/>
-    <row r="95" ht="12.75" customHeight="1"/>
-    <row r="96" ht="12.75" customHeight="1"/>
-    <row r="97" ht="12.75" customHeight="1"/>
-    <row r="98" ht="12.75" customHeight="1"/>
-    <row r="99" ht="12.75" customHeight="1"/>
-    <row r="100" ht="12.75" customHeight="1"/>
-    <row r="101" ht="12.75" customHeight="1"/>
-    <row r="102" ht="12.75" customHeight="1"/>
-    <row r="103" ht="12.75" customHeight="1"/>
-    <row r="104" ht="12.75" customHeight="1"/>
-    <row r="105" ht="12.75" customHeight="1"/>
-    <row r="106" ht="12.75" customHeight="1"/>
-    <row r="107" ht="12.75" customHeight="1"/>
-    <row r="108" ht="12.75" customHeight="1"/>
-    <row r="109" ht="12.75" customHeight="1"/>
-    <row r="110" ht="12.75" customHeight="1"/>
-    <row r="111" ht="12.75" customHeight="1"/>
-    <row r="112" ht="12.75" customHeight="1"/>
-    <row r="113" ht="12.75" customHeight="1"/>
-    <row r="114" ht="12.75" customHeight="1"/>
-    <row r="115" ht="12.75" customHeight="1"/>
-    <row r="116" ht="12.75" customHeight="1"/>
-    <row r="117" ht="12.75" customHeight="1"/>
-    <row r="118" ht="12.75" customHeight="1"/>
-    <row r="119" ht="12.75" customHeight="1"/>
-    <row r="120" ht="12.75" customHeight="1"/>
-    <row r="121" ht="12.75" customHeight="1"/>
-    <row r="122" ht="12.75" customHeight="1"/>
-    <row r="123" ht="12.75" customHeight="1"/>
-    <row r="124" ht="12.75" customHeight="1"/>
-    <row r="125" ht="12.75" customHeight="1"/>
-    <row r="126" ht="12.75" customHeight="1"/>
-    <row r="127" ht="12.75" customHeight="1"/>
-    <row r="128" ht="12.75" customHeight="1"/>
-    <row r="129" ht="12.75" customHeight="1"/>
-    <row r="130" ht="12.75" customHeight="1"/>
-    <row r="131" ht="12.75" customHeight="1"/>
-    <row r="132" ht="12.75" customHeight="1"/>
-    <row r="133" ht="12.75" customHeight="1"/>
-    <row r="134" ht="12.75" customHeight="1"/>
-    <row r="135" ht="12.75" customHeight="1"/>
-    <row r="136" ht="12.75" customHeight="1"/>
-    <row r="137" ht="12.75" customHeight="1"/>
-    <row r="138" ht="12.75" customHeight="1"/>
-    <row r="139" ht="12.75" customHeight="1"/>
-    <row r="140" ht="12.75" customHeight="1"/>
-    <row r="141" ht="12.75" customHeight="1"/>
-    <row r="142" ht="12.75" customHeight="1"/>
-    <row r="143" ht="12.75" customHeight="1"/>
-    <row r="144" ht="12.75" customHeight="1"/>
-    <row r="145" ht="12.75" customHeight="1"/>
-    <row r="146" ht="12.75" customHeight="1"/>
-    <row r="147" ht="12.75" customHeight="1"/>
-    <row r="148" ht="12.75" customHeight="1"/>
-    <row r="149" ht="12.75" customHeight="1"/>
-    <row r="150" ht="12.75" customHeight="1"/>
-    <row r="151" ht="12.75" customHeight="1"/>
-    <row r="152" ht="12.75" customHeight="1"/>
-    <row r="153" ht="12.75" customHeight="1"/>
-    <row r="154" ht="12.75" customHeight="1"/>
-    <row r="155" ht="12.75" customHeight="1"/>
-    <row r="156" ht="12.75" customHeight="1"/>
-    <row r="157" ht="12.75" customHeight="1"/>
-    <row r="158" ht="12.75" customHeight="1"/>
-    <row r="159" ht="12.75" customHeight="1"/>
-    <row r="160" ht="12.75" customHeight="1"/>
-    <row r="161" ht="12.75" customHeight="1"/>
-    <row r="162" ht="12.75" customHeight="1"/>
-    <row r="163" ht="12.75" customHeight="1"/>
-    <row r="164" ht="12.75" customHeight="1"/>
-    <row r="165" ht="12.75" customHeight="1"/>
-    <row r="166" ht="12.75" customHeight="1"/>
-    <row r="167" ht="12.75" customHeight="1"/>
-    <row r="168" ht="12.75" customHeight="1"/>
-    <row r="169" ht="12.75" customHeight="1"/>
-    <row r="170" ht="12.75" customHeight="1"/>
-    <row r="171" ht="12.75" customHeight="1"/>
-    <row r="172" ht="12.75" customHeight="1"/>
-    <row r="173" ht="12.75" customHeight="1"/>
-    <row r="174" ht="12.75" customHeight="1"/>
-    <row r="175" ht="12.75" customHeight="1"/>
-    <row r="176" ht="12.75" customHeight="1"/>
-    <row r="177" ht="12.75" customHeight="1"/>
-    <row r="178" ht="12.75" customHeight="1"/>
-    <row r="179" ht="12.75" customHeight="1"/>
-    <row r="180" ht="12.75" customHeight="1"/>
-    <row r="181" ht="12.75" customHeight="1"/>
-    <row r="182" ht="12.75" customHeight="1"/>
-    <row r="183" ht="12.75" customHeight="1"/>
-    <row r="184" ht="12.75" customHeight="1"/>
-    <row r="185" ht="12.75" customHeight="1"/>
-    <row r="186" ht="12.75" customHeight="1"/>
-    <row r="187" ht="12.75" customHeight="1"/>
-    <row r="188" ht="12.75" customHeight="1"/>
-    <row r="189" ht="12.75" customHeight="1"/>
-    <row r="190" ht="12.75" customHeight="1"/>
-    <row r="191" ht="12.75" customHeight="1"/>
-    <row r="192" ht="12.75" customHeight="1"/>
-    <row r="193" ht="12.75" customHeight="1"/>
-    <row r="194" ht="12.75" customHeight="1"/>
-    <row r="195" ht="12.75" customHeight="1"/>
-    <row r="196" ht="12.75" customHeight="1"/>
-    <row r="197" ht="12.75" customHeight="1"/>
-    <row r="198" ht="12.75" customHeight="1"/>
-    <row r="199" ht="12.75" customHeight="1"/>
-    <row r="200" ht="12.75" customHeight="1"/>
-    <row r="201" ht="12.75" customHeight="1"/>
-    <row r="202" ht="12.75" customHeight="1"/>
-    <row r="203" ht="12.75" customHeight="1"/>
-    <row r="204" ht="12.75" customHeight="1"/>
-    <row r="205" ht="12.75" customHeight="1"/>
-    <row r="206" ht="12.75" customHeight="1"/>
-    <row r="207" ht="12.75" customHeight="1"/>
-    <row r="208" ht="12.75" customHeight="1"/>
-    <row r="209" ht="12.75" customHeight="1"/>
-    <row r="210" ht="12.75" customHeight="1"/>
-    <row r="211" ht="12.75" customHeight="1"/>
-    <row r="212" ht="12.75" customHeight="1"/>
-    <row r="213" ht="12.75" customHeight="1"/>
-    <row r="214" ht="12.75" customHeight="1"/>
-    <row r="215" ht="12.75" customHeight="1"/>
-    <row r="216" ht="12.75" customHeight="1"/>
-    <row r="217" ht="12.75" customHeight="1"/>
-    <row r="218" ht="12.75" customHeight="1"/>
-    <row r="219" ht="12.75" customHeight="1"/>
-    <row r="220" ht="12.75" customHeight="1"/>
-    <row r="221" ht="12.75" customHeight="1"/>
-    <row r="222" ht="12.75" customHeight="1"/>
-    <row r="223" ht="12.75" customHeight="1"/>
-    <row r="224" ht="12.75" customHeight="1"/>
-    <row r="225" ht="12.75" customHeight="1"/>
-    <row r="226" ht="12.75" customHeight="1"/>
-    <row r="227" ht="12.75" customHeight="1"/>
-    <row r="228" ht="12.75" customHeight="1"/>
-    <row r="229" ht="12.75" customHeight="1"/>
-    <row r="230" ht="12.75" customHeight="1"/>
-    <row r="231" ht="12.75" customHeight="1"/>
-    <row r="232" ht="12.75" customHeight="1"/>
-    <row r="233" ht="12.75" customHeight="1"/>
-    <row r="234" ht="12.75" customHeight="1"/>
-    <row r="235" ht="12.75" customHeight="1"/>
-    <row r="236" ht="12.75" customHeight="1"/>
-    <row r="237" ht="12.75" customHeight="1"/>
-    <row r="238" ht="12.75" customHeight="1"/>
-    <row r="239" ht="12.75" customHeight="1"/>
-    <row r="240" ht="12.75" customHeight="1"/>
-    <row r="241" ht="12.75" customHeight="1"/>
-    <row r="242" ht="12.75" customHeight="1"/>
-    <row r="243" ht="12.75" customHeight="1"/>
-    <row r="244" ht="12.75" customHeight="1"/>
-    <row r="245" ht="12.75" customHeight="1"/>
-    <row r="246" ht="12.75" customHeight="1"/>
-    <row r="247" ht="12.75" customHeight="1"/>
-    <row r="248" ht="12.75" customHeight="1"/>
-    <row r="249" ht="12.75" customHeight="1"/>
-    <row r="250" ht="12.75" customHeight="1"/>
-    <row r="251" ht="12.75" customHeight="1"/>
-    <row r="252" ht="12.75" customHeight="1"/>
-    <row r="253" ht="12.75" customHeight="1"/>
-    <row r="254" ht="12.75" customHeight="1"/>
-    <row r="255" ht="12.75" customHeight="1"/>
-    <row r="256" ht="12.75" customHeight="1"/>
-    <row r="257" ht="12.75" customHeight="1"/>
-    <row r="258" ht="12.75" customHeight="1"/>
-    <row r="259" ht="12.75" customHeight="1"/>
-    <row r="260" ht="12.75" customHeight="1"/>
-    <row r="261" ht="12.75" customHeight="1"/>
-    <row r="262" ht="12.75" customHeight="1"/>
-    <row r="263" ht="12.75" customHeight="1"/>
-    <row r="264" ht="12.75" customHeight="1"/>
-    <row r="265" ht="12.75" customHeight="1"/>
-    <row r="266" ht="12.75" customHeight="1"/>
-    <row r="267" ht="12.75" customHeight="1"/>
-    <row r="268" ht="12.75" customHeight="1"/>
-    <row r="269" ht="12.75" customHeight="1"/>
-    <row r="270" ht="12.75" customHeight="1"/>
-    <row r="271" ht="12.75" customHeight="1"/>
-    <row r="272" ht="12.75" customHeight="1"/>
-    <row r="273" ht="12.75" customHeight="1"/>
-    <row r="274" ht="12.75" customHeight="1"/>
-    <row r="275" ht="12.75" customHeight="1"/>
-    <row r="276" ht="12.75" customHeight="1"/>
-    <row r="277" ht="12.75" customHeight="1"/>
-    <row r="278" ht="12.75" customHeight="1"/>
-    <row r="279" ht="12.75" customHeight="1"/>
-    <row r="280" ht="12.75" customHeight="1"/>
-    <row r="281" ht="12.75" customHeight="1"/>
-    <row r="282" ht="12.75" customHeight="1"/>
-    <row r="283" ht="12.75" customHeight="1"/>
-    <row r="284" ht="12.75" customHeight="1"/>
-    <row r="285" ht="12.75" customHeight="1"/>
-    <row r="286" ht="12.75" customHeight="1"/>
-    <row r="287" ht="12.75" customHeight="1"/>
-    <row r="288" ht="12.75" customHeight="1"/>
-    <row r="289" ht="12.75" customHeight="1"/>
-    <row r="290" ht="12.75" customHeight="1"/>
-    <row r="291" ht="12.75" customHeight="1"/>
-    <row r="292" ht="12.75" customHeight="1"/>
-    <row r="293" ht="12.75" customHeight="1"/>
-    <row r="294" ht="12.75" customHeight="1"/>
-    <row r="295" ht="12.75" customHeight="1"/>
-    <row r="296" ht="12.75" customHeight="1"/>
-    <row r="297" ht="12.75" customHeight="1"/>
-    <row r="298" ht="12.75" customHeight="1"/>
-    <row r="299" ht="12.75" customHeight="1"/>
-    <row r="300" ht="12.75" customHeight="1"/>
-    <row r="301" ht="12.75" customHeight="1"/>
-    <row r="302" ht="12.75" customHeight="1"/>
-    <row r="303" ht="12.75" customHeight="1"/>
-    <row r="304" ht="12.75" customHeight="1"/>
-    <row r="305" ht="12.75" customHeight="1"/>
-    <row r="306" ht="12.75" customHeight="1"/>
-    <row r="307" ht="12.75" customHeight="1"/>
-    <row r="308" ht="12.75" customHeight="1"/>
-    <row r="309" ht="12.75" customHeight="1"/>
-    <row r="310" ht="12.75" customHeight="1"/>
-    <row r="311" ht="12.75" customHeight="1"/>
-    <row r="312" ht="12.75" customHeight="1"/>
-    <row r="313" ht="12.75" customHeight="1"/>
-    <row r="314" ht="12.75" customHeight="1"/>
-    <row r="315" ht="12.75" customHeight="1"/>
-    <row r="316" ht="12.75" customHeight="1"/>
-    <row r="317" ht="12.75" customHeight="1"/>
-    <row r="318" ht="12.75" customHeight="1"/>
-    <row r="319" ht="12.75" customHeight="1"/>
-    <row r="320" ht="12.75" customHeight="1"/>
-    <row r="321" ht="12.75" customHeight="1"/>
-    <row r="322" ht="12.75" customHeight="1"/>
-    <row r="323" ht="12.75" customHeight="1"/>
-    <row r="324" ht="12.75" customHeight="1"/>
-    <row r="325" ht="12.75" customHeight="1"/>
-    <row r="326" ht="12.75" customHeight="1"/>
-    <row r="327" ht="12.75" customHeight="1"/>
-    <row r="328" ht="12.75" customHeight="1"/>
-    <row r="329" ht="12.75" customHeight="1"/>
-    <row r="330" ht="12.75" customHeight="1"/>
-    <row r="331" ht="12.75" customHeight="1"/>
-    <row r="332" ht="12.75" customHeight="1"/>
-    <row r="333" ht="12.75" customHeight="1"/>
-    <row r="334" ht="12.75" customHeight="1"/>
-    <row r="335" ht="12.75" customHeight="1"/>
-    <row r="336" ht="12.75" customHeight="1"/>
-    <row r="337" ht="12.75" customHeight="1"/>
-    <row r="338" ht="12.75" customHeight="1"/>
-    <row r="339" ht="12.75" customHeight="1"/>
-    <row r="340" ht="12.75" customHeight="1"/>
-    <row r="341" ht="12.75" customHeight="1"/>
-    <row r="342" ht="12.75" customHeight="1"/>
-    <row r="343" ht="12.75" customHeight="1"/>
-    <row r="344" ht="12.75" customHeight="1"/>
-    <row r="345" ht="12.75" customHeight="1"/>
-    <row r="346" ht="12.75" customHeight="1"/>
-    <row r="347" ht="12.75" customHeight="1"/>
-    <row r="348" ht="12.75" customHeight="1"/>
-    <row r="349" ht="12.75" customHeight="1"/>
-    <row r="350" ht="12.75" customHeight="1"/>
-    <row r="351" ht="12.75" customHeight="1"/>
-    <row r="352" ht="12.75" customHeight="1"/>
-    <row r="353" ht="12.75" customHeight="1"/>
-    <row r="354" ht="12.75" customHeight="1"/>
-    <row r="355" ht="12.75" customHeight="1"/>
-    <row r="356" ht="12.75" customHeight="1"/>
-    <row r="357" ht="12.75" customHeight="1"/>
-    <row r="358" ht="12.75" customHeight="1"/>
-    <row r="359" ht="12.75" customHeight="1"/>
-    <row r="360" ht="12.75" customHeight="1"/>
-    <row r="361" ht="12.75" customHeight="1"/>
-    <row r="362" ht="12.75" customHeight="1"/>
-    <row r="363" ht="12.75" customHeight="1"/>
-    <row r="364" ht="12.75" customHeight="1"/>
-    <row r="365" ht="12.75" customHeight="1"/>
-    <row r="366" ht="12.75" customHeight="1"/>
-    <row r="367" ht="12.75" customHeight="1"/>
-    <row r="368" ht="12.75" customHeight="1"/>
-    <row r="369" ht="12.75" customHeight="1"/>
-    <row r="370" ht="12.75" customHeight="1"/>
-    <row r="371" ht="12.75" customHeight="1"/>
-    <row r="372" ht="12.75" customHeight="1"/>
-    <row r="373" ht="12.75" customHeight="1"/>
-    <row r="374" ht="12.75" customHeight="1"/>
-    <row r="375" ht="12.75" customHeight="1"/>
-    <row r="376" ht="12.75" customHeight="1"/>
-    <row r="377" ht="12.75" customHeight="1"/>
-    <row r="378" ht="12.75" customHeight="1"/>
-    <row r="379" ht="12.75" customHeight="1"/>
-    <row r="380" ht="12.75" customHeight="1"/>
-    <row r="381" ht="12.75" customHeight="1"/>
-    <row r="382" ht="12.75" customHeight="1"/>
-    <row r="383" ht="12.75" customHeight="1"/>
-    <row r="384" ht="12.75" customHeight="1"/>
-    <row r="385" ht="12.75" customHeight="1"/>
-    <row r="386" ht="12.75" customHeight="1"/>
-    <row r="387" ht="12.75" customHeight="1"/>
-    <row r="388" ht="12.75" customHeight="1"/>
-    <row r="389" ht="12.75" customHeight="1"/>
-    <row r="390" ht="12.75" customHeight="1"/>
-    <row r="391" ht="12.75" customHeight="1"/>
-    <row r="392" ht="12.75" customHeight="1"/>
-    <row r="393" ht="12.75" customHeight="1"/>
-    <row r="394" ht="12.75" customHeight="1"/>
-    <row r="395" ht="12.75" customHeight="1"/>
-    <row r="396" ht="12.75" customHeight="1"/>
-    <row r="397" ht="12.75" customHeight="1"/>
-    <row r="398" ht="12.75" customHeight="1"/>
-    <row r="399" ht="12.75" customHeight="1"/>
-    <row r="400" ht="12.75" customHeight="1"/>
-    <row r="401" ht="12.75" customHeight="1"/>
-    <row r="402" ht="12.75" customHeight="1"/>
-    <row r="403" ht="12.75" customHeight="1"/>
-    <row r="404" ht="12.75" customHeight="1"/>
-    <row r="405" ht="12.75" customHeight="1"/>
-    <row r="406" ht="12.75" customHeight="1"/>
-    <row r="407" ht="12.75" customHeight="1"/>
-    <row r="408" ht="12.75" customHeight="1"/>
-    <row r="409" ht="12.75" customHeight="1"/>
-    <row r="410" ht="12.75" customHeight="1"/>
-    <row r="411" ht="12.75" customHeight="1"/>
-    <row r="412" ht="12.75" customHeight="1"/>
-    <row r="413" ht="12.75" customHeight="1"/>
-    <row r="414" ht="12.75" customHeight="1"/>
-    <row r="415" ht="12.75" customHeight="1"/>
-    <row r="416" ht="12.75" customHeight="1"/>
-    <row r="417" ht="12.75" customHeight="1"/>
-    <row r="418" ht="12.75" customHeight="1"/>
-    <row r="419" ht="12.75" customHeight="1"/>
-    <row r="420" ht="12.75" customHeight="1"/>
-    <row r="421" ht="12.75" customHeight="1"/>
-    <row r="422" ht="12.75" customHeight="1"/>
-    <row r="423" ht="12.75" customHeight="1"/>
-    <row r="424" ht="12.75" customHeight="1"/>
-    <row r="425" ht="12.75" customHeight="1"/>
-    <row r="426" ht="12.75" customHeight="1"/>
-    <row r="427" ht="12.75" customHeight="1"/>
-    <row r="428" ht="12.75" customHeight="1"/>
-    <row r="429" ht="12.75" customHeight="1"/>
-    <row r="430" ht="12.75" customHeight="1"/>
-    <row r="431" ht="12.75" customHeight="1"/>
-    <row r="432" ht="12.75" customHeight="1"/>
-    <row r="433" ht="12.75" customHeight="1"/>
-    <row r="434" ht="12.75" customHeight="1"/>
-    <row r="435" ht="12.75" customHeight="1"/>
-    <row r="436" ht="12.75" customHeight="1"/>
-    <row r="437" ht="12.75" customHeight="1"/>
-    <row r="438" ht="12.75" customHeight="1"/>
-    <row r="439" ht="12.75" customHeight="1"/>
-    <row r="440" ht="12.75" customHeight="1"/>
-    <row r="441" ht="12.75" customHeight="1"/>
-    <row r="442" ht="12.75" customHeight="1"/>
-    <row r="443" ht="12.75" customHeight="1"/>
-    <row r="444" ht="12.75" customHeight="1"/>
-    <row r="445" ht="12.75" customHeight="1"/>
-    <row r="446" ht="12.75" customHeight="1"/>
-    <row r="447" ht="12.75" customHeight="1"/>
-    <row r="448" ht="12.75" customHeight="1"/>
-    <row r="449" ht="12.75" customHeight="1"/>
-    <row r="450" ht="12.75" customHeight="1"/>
-    <row r="451" ht="12.75" customHeight="1"/>
-    <row r="452" ht="12.75" customHeight="1"/>
-    <row r="453" ht="12.75" customHeight="1"/>
-    <row r="454" ht="12.75" customHeight="1"/>
-    <row r="455" ht="12.75" customHeight="1"/>
-    <row r="456" ht="12.75" customHeight="1"/>
-    <row r="457" ht="12.75" customHeight="1"/>
-    <row r="458" ht="12.75" customHeight="1"/>
-    <row r="459" ht="12.75" customHeight="1"/>
-    <row r="460" ht="12.75" customHeight="1"/>
-    <row r="461" ht="12.75" customHeight="1"/>
-    <row r="462" ht="12.75" customHeight="1"/>
-    <row r="463" ht="12.75" customHeight="1"/>
-    <row r="464" ht="12.75" customHeight="1"/>
-    <row r="465" ht="12.75" customHeight="1"/>
-    <row r="466" ht="12.75" customHeight="1"/>
-    <row r="467" ht="12.75" customHeight="1"/>
-    <row r="468" ht="12.75" customHeight="1"/>
-    <row r="469" ht="12.75" customHeight="1"/>
-    <row r="470" ht="12.75" customHeight="1"/>
-    <row r="471" ht="12.75" customHeight="1"/>
-    <row r="472" ht="12.75" customHeight="1"/>
-    <row r="473" ht="12.75" customHeight="1"/>
-    <row r="474" ht="12.75" customHeight="1"/>
-    <row r="475" ht="12.75" customHeight="1"/>
-    <row r="476" ht="12.75" customHeight="1"/>
-    <row r="477" ht="12.75" customHeight="1"/>
-    <row r="478" ht="12.75" customHeight="1"/>
-    <row r="479" ht="12.75" customHeight="1"/>
-    <row r="480" ht="12.75" customHeight="1"/>
-    <row r="481" ht="12.75" customHeight="1"/>
-    <row r="482" ht="12.75" customHeight="1"/>
-    <row r="483" ht="12.75" customHeight="1"/>
-    <row r="484" ht="12.75" customHeight="1"/>
-    <row r="485" ht="12.75" customHeight="1"/>
-    <row r="486" ht="12.75" customHeight="1"/>
-    <row r="487" ht="12.75" customHeight="1"/>
-    <row r="488" ht="12.75" customHeight="1"/>
-    <row r="489" ht="12.75" customHeight="1"/>
-    <row r="490" ht="12.75" customHeight="1"/>
-    <row r="491" ht="12.75" customHeight="1"/>
-    <row r="492" ht="12.75" customHeight="1"/>
-    <row r="493" ht="12.75" customHeight="1"/>
-    <row r="494" ht="12.75" customHeight="1"/>
-    <row r="495" ht="12.75" customHeight="1"/>
-    <row r="496" ht="12.75" customHeight="1"/>
-    <row r="497" ht="12.75" customHeight="1"/>
-    <row r="498" ht="12.75" customHeight="1"/>
-    <row r="499" ht="12.75" customHeight="1"/>
-    <row r="500" ht="12.75" customHeight="1"/>
-    <row r="501" ht="12.75" customHeight="1"/>
-    <row r="502" ht="12.75" customHeight="1"/>
-    <row r="503" ht="12.75" customHeight="1"/>
-    <row r="504" ht="12.75" customHeight="1"/>
-    <row r="505" ht="12.75" customHeight="1"/>
-    <row r="506" ht="12.75" customHeight="1"/>
-    <row r="507" ht="12.75" customHeight="1"/>
-    <row r="508" ht="12.75" customHeight="1"/>
-    <row r="509" ht="12.75" customHeight="1"/>
-    <row r="510" ht="12.75" customHeight="1"/>
-    <row r="511" ht="12.75" customHeight="1"/>
-    <row r="512" ht="12.75" customHeight="1"/>
-    <row r="513" ht="12.75" customHeight="1"/>
-    <row r="514" ht="12.75" customHeight="1"/>
-    <row r="515" ht="12.75" customHeight="1"/>
-    <row r="516" ht="12.75" customHeight="1"/>
-    <row r="517" ht="12.75" customHeight="1"/>
-    <row r="518" ht="12.75" customHeight="1"/>
-    <row r="519" ht="12.75" customHeight="1"/>
-    <row r="520" ht="12.75" customHeight="1"/>
-    <row r="521" ht="12.75" customHeight="1"/>
-    <row r="522" ht="12.75" customHeight="1"/>
-    <row r="523" ht="12.75" customHeight="1"/>
-    <row r="524" ht="12.75" customHeight="1"/>
-    <row r="525" ht="12.75" customHeight="1"/>
-    <row r="526" ht="12.75" customHeight="1"/>
-    <row r="527" ht="12.75" customHeight="1"/>
-    <row r="528" ht="12.75" customHeight="1"/>
-    <row r="529" ht="12.75" customHeight="1"/>
-    <row r="530" ht="12.75" customHeight="1"/>
-    <row r="531" ht="12.75" customHeight="1"/>
-    <row r="532" ht="12.75" customHeight="1"/>
-    <row r="533" ht="12.75" customHeight="1"/>
-    <row r="534" ht="12.75" customHeight="1"/>
-    <row r="535" ht="12.75" customHeight="1"/>
-    <row r="536" ht="12.75" customHeight="1"/>
-    <row r="537" ht="12.75" customHeight="1"/>
-    <row r="538" ht="12.75" customHeight="1"/>
-    <row r="539" ht="12.75" customHeight="1"/>
-    <row r="540" ht="12.75" customHeight="1"/>
-    <row r="541" ht="12.75" customHeight="1"/>
-    <row r="542" ht="12.75" customHeight="1"/>
-    <row r="543" ht="12.75" customHeight="1"/>
-    <row r="544" ht="12.75" customHeight="1"/>
-    <row r="545" ht="12.75" customHeight="1"/>
-    <row r="546" ht="12.75" customHeight="1"/>
-    <row r="547" ht="12.75" customHeight="1"/>
-    <row r="548" ht="12.75" customHeight="1"/>
-    <row r="549" ht="12.75" customHeight="1"/>
-    <row r="550" ht="12.75" customHeight="1"/>
-    <row r="551" ht="12.75" customHeight="1"/>
-    <row r="552" ht="12.75" customHeight="1"/>
-    <row r="553" ht="12.75" customHeight="1"/>
-    <row r="554" ht="12.75" customHeight="1"/>
-    <row r="555" ht="12.75" customHeight="1"/>
-    <row r="556" ht="12.75" customHeight="1"/>
-    <row r="557" ht="12.75" customHeight="1"/>
-    <row r="558" ht="12.75" customHeight="1"/>
-    <row r="559" ht="12.75" customHeight="1"/>
-    <row r="560" ht="12.75" customHeight="1"/>
-    <row r="561" ht="12.75" customHeight="1"/>
-    <row r="562" ht="12.75" customHeight="1"/>
-    <row r="563" ht="12.75" customHeight="1"/>
-    <row r="564" ht="12.75" customHeight="1"/>
-    <row r="565" ht="12.75" customHeight="1"/>
-    <row r="566" ht="12.75" customHeight="1"/>
-    <row r="567" ht="12.75" customHeight="1"/>
-    <row r="568" ht="12.75" customHeight="1"/>
-    <row r="569" ht="12.75" customHeight="1"/>
-    <row r="570" ht="12.75" customHeight="1"/>
-    <row r="571" ht="12.75" customHeight="1"/>
-    <row r="572" ht="12.75" customHeight="1"/>
-    <row r="573" ht="12.75" customHeight="1"/>
-    <row r="574" ht="12.75" customHeight="1"/>
-    <row r="575" ht="12.75" customHeight="1"/>
-    <row r="576" ht="12.75" customHeight="1"/>
-    <row r="577" ht="12.75" customHeight="1"/>
-    <row r="578" ht="12.75" customHeight="1"/>
-    <row r="579" ht="12.75" customHeight="1"/>
-    <row r="580" ht="12.75" customHeight="1"/>
-    <row r="581" ht="12.75" customHeight="1"/>
-    <row r="582" ht="12.75" customHeight="1"/>
-    <row r="583" ht="12.75" customHeight="1"/>
-    <row r="584" ht="12.75" customHeight="1"/>
-    <row r="585" ht="12.75" customHeight="1"/>
-    <row r="586" ht="12.75" customHeight="1"/>
-    <row r="587" ht="12.75" customHeight="1"/>
-    <row r="588" ht="12.75" customHeight="1"/>
-    <row r="589" ht="12.75" customHeight="1"/>
-    <row r="590" ht="12.75" customHeight="1"/>
-    <row r="591" ht="12.75" customHeight="1"/>
-    <row r="592" ht="12.75" customHeight="1"/>
-    <row r="593" ht="12.75" customHeight="1"/>
-    <row r="594" ht="12.75" customHeight="1"/>
-    <row r="595" ht="12.75" customHeight="1"/>
-    <row r="596" ht="12.75" customHeight="1"/>
-    <row r="597" ht="12.75" customHeight="1"/>
-    <row r="598" ht="12.75" customHeight="1"/>
-    <row r="599" ht="12.75" customHeight="1"/>
-    <row r="600" ht="12.75" customHeight="1"/>
-    <row r="601" ht="12.75" customHeight="1"/>
-    <row r="602" ht="12.75" customHeight="1"/>
-    <row r="603" ht="12.75" customHeight="1"/>
-    <row r="604" ht="12.75" customHeight="1"/>
-    <row r="605" ht="12.75" customHeight="1"/>
-    <row r="606" ht="12.75" customHeight="1"/>
-    <row r="607" ht="12.75" customHeight="1"/>
-    <row r="608" ht="12.75" customHeight="1"/>
-    <row r="609" ht="12.75" customHeight="1"/>
-    <row r="610" ht="12.75" customHeight="1"/>
-    <row r="611" ht="12.75" customHeight="1"/>
-    <row r="612" ht="12.75" customHeight="1"/>
-    <row r="613" ht="12.75" customHeight="1"/>
-    <row r="614" ht="12.75" customHeight="1"/>
-    <row r="615" ht="12.75" customHeight="1"/>
-    <row r="616" ht="12.75" customHeight="1"/>
-    <row r="617" ht="12.75" customHeight="1"/>
-    <row r="618" ht="12.75" customHeight="1"/>
-    <row r="619" ht="12.75" customHeight="1"/>
-    <row r="620" ht="12.75" customHeight="1"/>
-    <row r="621" ht="12.75" customHeight="1"/>
-    <row r="622" ht="12.75" customHeight="1"/>
-    <row r="623" ht="12.75" customHeight="1"/>
-    <row r="624" ht="12.75" customHeight="1"/>
-    <row r="625" ht="12.75" customHeight="1"/>
-    <row r="626" ht="12.75" customHeight="1"/>
-    <row r="627" ht="12.75" customHeight="1"/>
-    <row r="628" ht="12.75" customHeight="1"/>
-    <row r="629" ht="12.75" customHeight="1"/>
-    <row r="630" ht="12.75" customHeight="1"/>
-    <row r="631" ht="12.75" customHeight="1"/>
-    <row r="632" ht="12.75" customHeight="1"/>
-    <row r="633" ht="12.75" customHeight="1"/>
-    <row r="634" ht="12.75" customHeight="1"/>
-    <row r="635" ht="12.75" customHeight="1"/>
-    <row r="636" ht="12.75" customHeight="1"/>
-    <row r="637" ht="12.75" customHeight="1"/>
-    <row r="638" ht="12.75" customHeight="1"/>
-    <row r="639" ht="12.75" customHeight="1"/>
-    <row r="640" ht="12.75" customHeight="1"/>
-    <row r="641" ht="12.75" customHeight="1"/>
-    <row r="642" ht="12.75" customHeight="1"/>
-    <row r="643" ht="12.75" customHeight="1"/>
-    <row r="644" ht="12.75" customHeight="1"/>
-    <row r="645" ht="12.75" customHeight="1"/>
-    <row r="646" ht="12.75" customHeight="1"/>
-    <row r="647" ht="12.75" customHeight="1"/>
-    <row r="648" ht="12.75" customHeight="1"/>
-    <row r="649" ht="12.75" customHeight="1"/>
-    <row r="650" ht="12.75" customHeight="1"/>
-    <row r="651" ht="12.75" customHeight="1"/>
-    <row r="652" ht="12.75" customHeight="1"/>
-    <row r="653" ht="12.75" customHeight="1"/>
-    <row r="654" ht="12.75" customHeight="1"/>
-    <row r="655" ht="12.75" customHeight="1"/>
-    <row r="656" ht="12.75" customHeight="1"/>
-    <row r="657" ht="12.75" customHeight="1"/>
-    <row r="658" ht="12.75" customHeight="1"/>
-    <row r="659" ht="12.75" customHeight="1"/>
-    <row r="660" ht="12.75" customHeight="1"/>
-    <row r="661" ht="12.75" customHeight="1"/>
-    <row r="662" ht="12.75" customHeight="1"/>
-    <row r="663" ht="12.75" customHeight="1"/>
-    <row r="664" ht="12.75" customHeight="1"/>
-    <row r="665" ht="12.75" customHeight="1"/>
-    <row r="666" ht="12.75" customHeight="1"/>
-    <row r="667" ht="12.75" customHeight="1"/>
-    <row r="668" ht="12.75" customHeight="1"/>
-    <row r="669" ht="12.75" customHeight="1"/>
-    <row r="670" ht="12.75" customHeight="1"/>
-    <row r="671" ht="12.75" customHeight="1"/>
-    <row r="672" ht="12.75" customHeight="1"/>
-    <row r="673" ht="12.75" customHeight="1"/>
-    <row r="674" ht="12.75" customHeight="1"/>
-    <row r="675" ht="12.75" customHeight="1"/>
-    <row r="676" ht="12.75" customHeight="1"/>
-    <row r="677" ht="12.75" customHeight="1"/>
-    <row r="678" ht="12.75" customHeight="1"/>
-    <row r="679" ht="12.75" customHeight="1"/>
-    <row r="680" ht="12.75" customHeight="1"/>
-    <row r="681" ht="12.75" customHeight="1"/>
-    <row r="682" ht="12.75" customHeight="1"/>
-    <row r="683" ht="12.75" customHeight="1"/>
-    <row r="684" ht="12.75" customHeight="1"/>
-    <row r="685" ht="12.75" customHeight="1"/>
-    <row r="686" ht="12.75" customHeight="1"/>
-    <row r="687" ht="12.75" customHeight="1"/>
-    <row r="688" ht="12.75" customHeight="1"/>
-    <row r="689" ht="12.75" customHeight="1"/>
-    <row r="690" ht="12.75" customHeight="1"/>
-    <row r="691" ht="12.75" customHeight="1"/>
-    <row r="692" ht="12.75" customHeight="1"/>
-    <row r="693" ht="12.75" customHeight="1"/>
-    <row r="694" ht="12.75" customHeight="1"/>
-    <row r="695" ht="12.75" customHeight="1"/>
-    <row r="696" ht="12.75" customHeight="1"/>
-    <row r="697" ht="12.75" customHeight="1"/>
-    <row r="698" ht="12.75" customHeight="1"/>
-    <row r="699" ht="12.75" customHeight="1"/>
-    <row r="700" ht="12.75" customHeight="1"/>
-    <row r="701" ht="12.75" customHeight="1"/>
-    <row r="702" ht="12.75" customHeight="1"/>
-    <row r="703" ht="12.75" customHeight="1"/>
-    <row r="704" ht="12.75" customHeight="1"/>
-    <row r="705" ht="12.75" customHeight="1"/>
-    <row r="706" ht="12.75" customHeight="1"/>
-    <row r="707" ht="12.75" customHeight="1"/>
-    <row r="708" ht="12.75" customHeight="1"/>
-    <row r="709" ht="12.75" customHeight="1"/>
-    <row r="710" ht="12.75" customHeight="1"/>
-    <row r="711" ht="12.75" customHeight="1"/>
-    <row r="712" ht="12.75" customHeight="1"/>
-    <row r="713" ht="12.75" customHeight="1"/>
-    <row r="714" ht="12.75" customHeight="1"/>
-    <row r="715" ht="12.75" customHeight="1"/>
-    <row r="716" ht="12.75" customHeight="1"/>
-    <row r="717" ht="12.75" customHeight="1"/>
-    <row r="718" ht="12.75" customHeight="1"/>
-    <row r="719" ht="12.75" customHeight="1"/>
-    <row r="720" ht="12.75" customHeight="1"/>
-    <row r="721" ht="12.75" customHeight="1"/>
-    <row r="722" ht="12.75" customHeight="1"/>
-    <row r="723" ht="12.75" customHeight="1"/>
-    <row r="724" ht="12.75" customHeight="1"/>
-    <row r="725" ht="12.75" customHeight="1"/>
-    <row r="726" ht="12.75" customHeight="1"/>
-    <row r="727" ht="12.75" customHeight="1"/>
-    <row r="728" ht="12.75" customHeight="1"/>
-    <row r="729" ht="12.75" customHeight="1"/>
-    <row r="730" ht="12.75" customHeight="1"/>
-    <row r="731" ht="12.75" customHeight="1"/>
-    <row r="732" ht="12.75" customHeight="1"/>
-    <row r="733" ht="12.75" customHeight="1"/>
-    <row r="734" ht="12.75" customHeight="1"/>
-    <row r="735" ht="12.75" customHeight="1"/>
-    <row r="736" ht="12.75" customHeight="1"/>
-    <row r="737" ht="12.75" customHeight="1"/>
-    <row r="738" ht="12.75" customHeight="1"/>
-    <row r="739" ht="12.75" customHeight="1"/>
-    <row r="740" ht="12.75" customHeight="1"/>
-    <row r="741" ht="12.75" customHeight="1"/>
-    <row r="742" ht="12.75" customHeight="1"/>
-    <row r="743" ht="12.75" customHeight="1"/>
-    <row r="744" ht="12.75" customHeight="1"/>
-    <row r="745" ht="12.75" customHeight="1"/>
-    <row r="746" ht="12.75" customHeight="1"/>
-    <row r="747" ht="12.75" customHeight="1"/>
-    <row r="748" ht="12.75" customHeight="1"/>
-    <row r="749" ht="12.75" customHeight="1"/>
-    <row r="750" ht="12.75" customHeight="1"/>
-    <row r="751" ht="12.75" customHeight="1"/>
-    <row r="752" ht="12.75" customHeight="1"/>
-    <row r="753" ht="12.75" customHeight="1"/>
-    <row r="754" ht="12.75" customHeight="1"/>
-    <row r="755" ht="12.75" customHeight="1"/>
-    <row r="756" ht="12.75" customHeight="1"/>
-    <row r="757" ht="12.75" customHeight="1"/>
-    <row r="758" ht="12.75" customHeight="1"/>
-    <row r="759" ht="12.75" customHeight="1"/>
-    <row r="760" ht="12.75" customHeight="1"/>
-    <row r="761" ht="12.75" customHeight="1"/>
-    <row r="762" ht="12.75" customHeight="1"/>
-    <row r="763" ht="12.75" customHeight="1"/>
-    <row r="764" ht="12.75" customHeight="1"/>
-    <row r="765" ht="12.75" customHeight="1"/>
-    <row r="766" ht="12.75" customHeight="1"/>
-    <row r="767" ht="12.75" customHeight="1"/>
-    <row r="768" ht="12.75" customHeight="1"/>
-    <row r="769" ht="12.75" customHeight="1"/>
-    <row r="770" ht="12.75" customHeight="1"/>
-    <row r="771" ht="12.75" customHeight="1"/>
-    <row r="772" ht="12.75" customHeight="1"/>
-    <row r="773" ht="12.75" customHeight="1"/>
-    <row r="774" ht="12.75" customHeight="1"/>
-    <row r="775" ht="12.75" customHeight="1"/>
-    <row r="776" ht="12.75" customHeight="1"/>
-    <row r="777" ht="12.75" customHeight="1"/>
-    <row r="778" ht="12.75" customHeight="1"/>
-    <row r="779" ht="12.75" customHeight="1"/>
-    <row r="780" ht="12.75" customHeight="1"/>
-    <row r="781" ht="12.75" customHeight="1"/>
-    <row r="782" ht="12.75" customHeight="1"/>
-    <row r="783" ht="12.75" customHeight="1"/>
-    <row r="784" ht="12.75" customHeight="1"/>
-    <row r="785" ht="12.75" customHeight="1"/>
-    <row r="786" ht="12.75" customHeight="1"/>
-    <row r="787" ht="12.75" customHeight="1"/>
-    <row r="788" ht="12.75" customHeight="1"/>
-    <row r="789" ht="12.75" customHeight="1"/>
-    <row r="790" ht="12.75" customHeight="1"/>
-    <row r="791" ht="12.75" customHeight="1"/>
-    <row r="792" ht="12.75" customHeight="1"/>
-    <row r="793" ht="12.75" customHeight="1"/>
-    <row r="794" ht="12.75" customHeight="1"/>
-    <row r="795" ht="12.75" customHeight="1"/>
-    <row r="796" ht="12.75" customHeight="1"/>
-    <row r="797" ht="12.75" customHeight="1"/>
-    <row r="798" ht="12.75" customHeight="1"/>
-    <row r="799" ht="12.75" customHeight="1"/>
-    <row r="800" ht="12.75" customHeight="1"/>
-    <row r="801" ht="12.75" customHeight="1"/>
-    <row r="802" ht="12.75" customHeight="1"/>
-    <row r="803" ht="12.75" customHeight="1"/>
-    <row r="804" ht="12.75" customHeight="1"/>
-    <row r="805" ht="12.75" customHeight="1"/>
-    <row r="806" ht="12.75" customHeight="1"/>
-    <row r="807" ht="12.75" customHeight="1"/>
-    <row r="808" ht="12.75" customHeight="1"/>
-    <row r="809" ht="12.75" customHeight="1"/>
-    <row r="810" ht="12.75" customHeight="1"/>
-    <row r="811" ht="12.75" customHeight="1"/>
-    <row r="812" ht="12.75" customHeight="1"/>
-    <row r="813" ht="12.75" customHeight="1"/>
-    <row r="814" ht="12.75" customHeight="1"/>
-    <row r="815" ht="12.75" customHeight="1"/>
-    <row r="816" ht="12.75" customHeight="1"/>
-    <row r="817" ht="12.75" customHeight="1"/>
-    <row r="818" ht="12.75" customHeight="1"/>
-    <row r="819" ht="12.75" customHeight="1"/>
-    <row r="820" ht="12.75" customHeight="1"/>
-    <row r="821" ht="12.75" customHeight="1"/>
-    <row r="822" ht="12.75" customHeight="1"/>
-    <row r="823" ht="12.75" customHeight="1"/>
-    <row r="824" ht="12.75" customHeight="1"/>
-    <row r="825" ht="12.75" customHeight="1"/>
-    <row r="826" ht="12.75" customHeight="1"/>
-    <row r="827" ht="12.75" customHeight="1"/>
-    <row r="828" ht="12.75" customHeight="1"/>
-    <row r="829" ht="12.75" customHeight="1"/>
-    <row r="830" ht="12.75" customHeight="1"/>
-    <row r="831" ht="12.75" customHeight="1"/>
-    <row r="832" ht="12.75" customHeight="1"/>
-    <row r="833" ht="12.75" customHeight="1"/>
-    <row r="834" ht="12.75" customHeight="1"/>
-    <row r="835" ht="12.75" customHeight="1"/>
-    <row r="836" ht="12.75" customHeight="1"/>
-    <row r="837" ht="12.75" customHeight="1"/>
-    <row r="838" ht="12.75" customHeight="1"/>
-    <row r="839" ht="12.75" customHeight="1"/>
-    <row r="840" ht="12.75" customHeight="1"/>
-    <row r="841" ht="12.75" customHeight="1"/>
-    <row r="842" ht="12.75" customHeight="1"/>
-    <row r="843" ht="12.75" customHeight="1"/>
-    <row r="844" ht="12.75" customHeight="1"/>
-    <row r="845" ht="12.75" customHeight="1"/>
-    <row r="846" ht="12.75" customHeight="1"/>
-    <row r="847" ht="12.75" customHeight="1"/>
-    <row r="848" ht="12.75" customHeight="1"/>
-    <row r="849" ht="12.75" customHeight="1"/>
-    <row r="850" ht="12.75" customHeight="1"/>
-    <row r="851" ht="12.75" customHeight="1"/>
-    <row r="852" ht="12.75" customHeight="1"/>
-    <row r="853" ht="12.75" customHeight="1"/>
-    <row r="854" ht="12.75" customHeight="1"/>
-    <row r="855" ht="12.75" customHeight="1"/>
-    <row r="856" ht="12.75" customHeight="1"/>
-    <row r="857" ht="12.75" customHeight="1"/>
-    <row r="858" ht="12.75" customHeight="1"/>
-    <row r="859" ht="12.75" customHeight="1"/>
-    <row r="860" ht="12.75" customHeight="1"/>
-    <row r="861" ht="12.75" customHeight="1"/>
-    <row r="862" ht="12.75" customHeight="1"/>
-    <row r="863" ht="12.75" customHeight="1"/>
-    <row r="864" ht="12.75" customHeight="1"/>
-    <row r="865" ht="12.75" customHeight="1"/>
-    <row r="866" ht="12.75" customHeight="1"/>
-    <row r="867" ht="12.75" customHeight="1"/>
-    <row r="868" ht="12.75" customHeight="1"/>
-    <row r="869" ht="12.75" customHeight="1"/>
-    <row r="870" ht="12.75" customHeight="1"/>
-    <row r="871" ht="12.75" customHeight="1"/>
-    <row r="872" ht="12.75" customHeight="1"/>
-    <row r="873" ht="12.75" customHeight="1"/>
-    <row r="874" ht="12.75" customHeight="1"/>
-    <row r="875" ht="12.75" customHeight="1"/>
-    <row r="876" ht="12.75" customHeight="1"/>
-    <row r="877" ht="12.75" customHeight="1"/>
-    <row r="878" ht="12.75" customHeight="1"/>
-    <row r="879" ht="12.75" customHeight="1"/>
-    <row r="880" ht="12.75" customHeight="1"/>
-    <row r="881" ht="12.75" customHeight="1"/>
-    <row r="882" ht="12.75" customHeight="1"/>
-    <row r="883" ht="12.75" customHeight="1"/>
-    <row r="884" ht="12.75" customHeight="1"/>
-    <row r="885" ht="12.75" customHeight="1"/>
-    <row r="886" ht="12.75" customHeight="1"/>
-    <row r="887" ht="12.75" customHeight="1"/>
-    <row r="888" ht="12.75" customHeight="1"/>
-    <row r="889" ht="12.75" customHeight="1"/>
-    <row r="890" ht="12.75" customHeight="1"/>
-    <row r="891" ht="12.75" customHeight="1"/>
-    <row r="892" ht="12.75" customHeight="1"/>
-    <row r="893" ht="12.75" customHeight="1"/>
-    <row r="894" ht="12.75" customHeight="1"/>
-    <row r="895" ht="12.75" customHeight="1"/>
-    <row r="896" ht="12.75" customHeight="1"/>
-    <row r="897" ht="12.75" customHeight="1"/>
-    <row r="898" ht="12.75" customHeight="1"/>
-    <row r="899" ht="12.75" customHeight="1"/>
-    <row r="900" ht="12.75" customHeight="1"/>
-    <row r="901" ht="12.75" customHeight="1"/>
-    <row r="902" ht="12.75" customHeight="1"/>
-    <row r="903" ht="12.75" customHeight="1"/>
-    <row r="904" ht="12.75" customHeight="1"/>
-    <row r="905" ht="12.75" customHeight="1"/>
-    <row r="906" ht="12.75" customHeight="1"/>
-    <row r="907" ht="12.75" customHeight="1"/>
-    <row r="908" ht="12.75" customHeight="1"/>
-    <row r="909" ht="12.75" customHeight="1"/>
-    <row r="910" ht="12.75" customHeight="1"/>
-    <row r="911" ht="12.75" customHeight="1"/>
-    <row r="912" ht="12.75" customHeight="1"/>
-    <row r="913" ht="12.75" customHeight="1"/>
-    <row r="914" ht="12.75" customHeight="1"/>
-    <row r="915" ht="12.75" customHeight="1"/>
-    <row r="916" ht="12.75" customHeight="1"/>
-    <row r="917" ht="12.75" customHeight="1"/>
-    <row r="918" ht="12.75" customHeight="1"/>
-    <row r="919" ht="12.75" customHeight="1"/>
-    <row r="920" ht="12.75" customHeight="1"/>
-    <row r="921" ht="12.75" customHeight="1"/>
-    <row r="922" ht="12.75" customHeight="1"/>
-    <row r="923" ht="12.75" customHeight="1"/>
-    <row r="924" ht="12.75" customHeight="1"/>
-    <row r="925" ht="12.75" customHeight="1"/>
-    <row r="926" ht="12.75" customHeight="1"/>
-    <row r="927" ht="12.75" customHeight="1"/>
-    <row r="928" ht="12.75" customHeight="1"/>
-    <row r="929" ht="12.75" customHeight="1"/>
-    <row r="930" ht="12.75" customHeight="1"/>
-    <row r="931" ht="12.75" customHeight="1"/>
-    <row r="932" ht="12.75" customHeight="1"/>
-    <row r="933" ht="12.75" customHeight="1"/>
-    <row r="934" ht="12.75" customHeight="1"/>
-    <row r="935" ht="12.75" customHeight="1"/>
-    <row r="936" ht="12.75" customHeight="1"/>
-    <row r="937" ht="12.75" customHeight="1"/>
-    <row r="938" ht="12.75" customHeight="1"/>
-    <row r="939" ht="12.75" customHeight="1"/>
-    <row r="940" ht="12.75" customHeight="1"/>
-    <row r="941" ht="12.75" customHeight="1"/>
-    <row r="942" ht="12.75" customHeight="1"/>
-    <row r="943" ht="12.75" customHeight="1"/>
-    <row r="944" ht="12.75" customHeight="1"/>
-    <row r="945" ht="12.75" customHeight="1"/>
-    <row r="946" ht="12.75" customHeight="1"/>
-    <row r="947" ht="12.75" customHeight="1"/>
-    <row r="948" ht="12.75" customHeight="1"/>
-    <row r="949" ht="12.75" customHeight="1"/>
-    <row r="950" ht="12.75" customHeight="1"/>
-    <row r="951" ht="12.75" customHeight="1"/>
-    <row r="952" ht="12.75" customHeight="1"/>
-    <row r="953" ht="12.75" customHeight="1"/>
-    <row r="954" ht="12.75" customHeight="1"/>
-    <row r="955" ht="12.75" customHeight="1"/>
-    <row r="956" ht="12.75" customHeight="1"/>
-    <row r="957" ht="12.75" customHeight="1"/>
-    <row r="958" ht="12.75" customHeight="1"/>
-    <row r="959" ht="12.75" customHeight="1"/>
-    <row r="960" ht="12.75" customHeight="1"/>
-    <row r="961" ht="12.75" customHeight="1"/>
-    <row r="962" ht="12.75" customHeight="1"/>
-    <row r="963" ht="12.75" customHeight="1"/>
-    <row r="964" ht="12.75" customHeight="1"/>
-    <row r="965" ht="12.75" customHeight="1"/>
-    <row r="966" ht="12.75" customHeight="1"/>
-    <row r="967" ht="12.75" customHeight="1"/>
-    <row r="968" ht="12.75" customHeight="1"/>
-    <row r="969" ht="12.75" customHeight="1"/>
-    <row r="970" ht="12.75" customHeight="1"/>
-    <row r="971" ht="12.75" customHeight="1"/>
-    <row r="972" ht="12.75" customHeight="1"/>
-    <row r="973" ht="12.75" customHeight="1"/>
-    <row r="974" ht="12.75" customHeight="1"/>
-    <row r="975" ht="12.75" customHeight="1"/>
-    <row r="976" ht="12.75" customHeight="1"/>
-    <row r="977" ht="12.75" customHeight="1"/>
-    <row r="978" ht="12.75" customHeight="1"/>
-    <row r="979" ht="12.75" customHeight="1"/>
-    <row r="980" ht="12.75" customHeight="1"/>
-    <row r="981" ht="12.75" customHeight="1"/>
-    <row r="982" ht="12.75" customHeight="1"/>
-    <row r="983" ht="12.75" customHeight="1"/>
-    <row r="984" ht="12.75" customHeight="1"/>
-    <row r="985" ht="12.75" customHeight="1"/>
-    <row r="986" ht="12.75" customHeight="1"/>
-    <row r="987" ht="12.75" customHeight="1"/>
-    <row r="988" ht="12.75" customHeight="1"/>
-    <row r="989" ht="12.75" customHeight="1"/>
-    <row r="990" ht="12.75" customHeight="1"/>
-    <row r="991" ht="12.75" customHeight="1"/>
-    <row r="992" ht="12.75" customHeight="1"/>
-    <row r="993" ht="12.75" customHeight="1"/>
-    <row r="994" ht="12.75" customHeight="1"/>
-    <row r="995" ht="12.75" customHeight="1"/>
-    <row r="996" ht="12.75" customHeight="1"/>
-    <row r="997" ht="12.75" customHeight="1"/>
-    <row r="998" ht="12.75" customHeight="1"/>
-    <row r="999" ht="12.75" customHeight="1"/>
-    <row r="1000" ht="12.75" customHeight="1"/>
-  </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins bottom="0.3" footer="0.0" header="0.0" left="0.3" right="0.3" top="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>